<commit_message>
Added results png files for adjoint vs. direct study
</commit_message>
<xml_diff>
--- a/doc/hmcsa_adjoint_vs_direct/direct_vs_adjoint.xlsx
+++ b/doc/hmcsa_adjoint_vs_direct/direct_vs_adjoint.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="0" windowWidth="25820" windowHeight="23480" tabRatio="500"/>
+    <workbookView xWindow="12560" yWindow="0" windowWidth="25820" windowHeight="23480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Timing Study" sheetId="1" r:id="rId1"/>
+    <sheet name="Convergence Study" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>problem parameters</t>
   </si>
@@ -80,6 +81,24 @@
   <si>
     <t>Direct 9 Point</t>
   </si>
+  <si>
+    <t>Convergence study for the Laplace equation using MCSA as the solver. (one time step with the heat equation)</t>
+  </si>
+  <si>
+    <t>Nx</t>
+  </si>
+  <si>
+    <t>Ny</t>
+  </si>
+  <si>
+    <t>I am reporting the infinity norm of the residual</t>
+  </si>
+  <si>
+    <t>Iteration</t>
+  </si>
+  <si>
+    <t>inf_norm</t>
+  </si>
 </sst>
 </file>
 
@@ -135,7 +154,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -143,20 +162,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -213,7 +257,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$15</c:f>
+              <c:f>'Timing Study'!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -222,9 +266,30 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$21</c:f>
+              <c:f>'Timing Study'!$A$17:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -248,7 +313,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$B$21</c:f>
+              <c:f>'Timing Study'!$B$17:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -277,7 +342,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$15</c:f>
+              <c:f>'Timing Study'!$D$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -286,9 +351,30 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$21</c:f>
+              <c:f>'Timing Study'!$A$17:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -312,7 +398,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$21</c:f>
+              <c:f>'Timing Study'!$D$17:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -341,7 +427,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$15</c:f>
+              <c:f>'Timing Study'!$H$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -350,9 +436,30 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$21</c:f>
+              <c:f>'Timing Study'!$G$17:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -376,7 +483,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$17:$H$21</c:f>
+              <c:f>'Timing Study'!$H$17:$H$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -405,7 +512,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$15</c:f>
+              <c:f>'Timing Study'!$J$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -414,9 +521,30 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$21</c:f>
+              <c:f>'Timing Study'!$G$17:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -440,7 +568,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$17:$J$21</c:f>
+              <c:f>'Timing Study'!$J$17:$J$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -472,13 +600,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2141175400"/>
-        <c:axId val="2140669720"/>
+        <c:axId val="2121052280"/>
+        <c:axId val="2121057976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2141175400"/>
+        <c:axId val="2121052280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="101.0"/>
+          <c:min val="20.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -509,13 +639,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140669720"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="2121057976"/>
+        <c:crossesAt val="0.01"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2140669720"/>
+        <c:axId val="2121057976"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -544,7 +675,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141175400"/>
+        <c:crossAx val="2121052280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -615,7 +746,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$15</c:f>
+              <c:f>'Timing Study'!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -624,9 +755,30 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$21</c:f>
+              <c:f>'Timing Study'!$A$17:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -650,7 +802,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$21</c:f>
+              <c:f>'Timing Study'!$C$17:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -679,7 +831,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$15</c:f>
+              <c:f>'Timing Study'!$D$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -688,9 +840,30 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$21</c:f>
+              <c:f>'Timing Study'!$A$17:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -714,7 +887,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$17:$E$21</c:f>
+              <c:f>'Timing Study'!$E$17:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -743,7 +916,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$15</c:f>
+              <c:f>'Timing Study'!$H$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -752,9 +925,30 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$21</c:f>
+              <c:f>'Timing Study'!$G$17:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -778,7 +972,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$17:$I$21</c:f>
+              <c:f>'Timing Study'!$I$17:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -807,7 +1001,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$15</c:f>
+              <c:f>'Timing Study'!$J$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -816,9 +1010,34 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$21</c:f>
+              <c:f>'Timing Study'!$G$17:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -842,7 +1061,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$17:$K$21</c:f>
+              <c:f>'Timing Study'!$K$17:$K$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -874,13 +1093,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2137105816"/>
-        <c:axId val="2140693224"/>
+        <c:axId val="2121099768"/>
+        <c:axId val="2121105576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2137105816"/>
+        <c:axId val="2121099768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="101.0"/>
+          <c:min val="20.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -912,12 +1133,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140693224"/>
+        <c:crossAx val="2121105576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2140693224"/>
+        <c:axId val="2121105576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40.0"/>
@@ -948,7 +1169,1680 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137105816"/>
+        <c:crossAx val="2121099768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Residual</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Inf_Norm vs. Iterations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Convergence Study'!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Adjoint 5 Point</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Convergence Study'!$A$18:$A$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="61"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Convergence Study'!$B$18:$B$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="61"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0655</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.51008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.827511</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45779</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.322095</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.191576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.137312</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0919966</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0632601</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0452385</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0322903</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0234289</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0173023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0125367</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.00932899</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.00675807</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0050668</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.00367012</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.00277274</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.00200733</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.00156768</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.00118507</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.000922597</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.000702234</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.000543244</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.000416313</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.00032022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.000248303</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.000190668</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.000148665</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.000115014</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="0.00E+00">
+                  <c:v>8.9019E-5</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="0.00E+00">
+                  <c:v>6.93523E-5</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0.00E+00">
+                  <c:v>5.33285E-5</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0.00E+00">
+                  <c:v>4.18196E-5</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0.00E+00">
+                  <c:v>3.19699E-5</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0.00E+00">
+                  <c:v>2.52247E-5</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="0.00E+00">
+                  <c:v>1.93258E-5</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="0.00E+00">
+                  <c:v>1.52225E-5</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="0.00E+00">
+                  <c:v>1.17774E-5</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="0.00E+00">
+                  <c:v>9.19214E-6</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="0.00E+00">
+                  <c:v>7.17577E-6</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="0.00E+00">
+                  <c:v>5.55471E-6</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="0.00E+00">
+                  <c:v>4.37198E-6</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="0.00E+00">
+                  <c:v>3.35927E-6</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="0.00E+00">
+                  <c:v>2.66406E-6</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="0.00E+00">
+                  <c:v>2.05042E-6</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="0.00E+00">
+                  <c:v>1.62373E-6</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="0.00E+00">
+                  <c:v>1.2557E-6</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="0.00E+00">
+                  <c:v>9.89973E-7</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="0.00E+00">
+                  <c:v>7.69065E-7</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="0.00E+00">
+                  <c:v>6.03812E-7</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="0.00E+00">
+                  <c:v>4.71096E-7</c:v>
+                </c:pt>
+                <c:pt idx="54" formatCode="0.00E+00">
+                  <c:v>3.68442E-7</c:v>
+                </c:pt>
+                <c:pt idx="55" formatCode="0.00E+00">
+                  <c:v>2.88638E-7</c:v>
+                </c:pt>
+                <c:pt idx="56" formatCode="0.00E+00">
+                  <c:v>2.2493E-7</c:v>
+                </c:pt>
+                <c:pt idx="57" formatCode="0.00E+00">
+                  <c:v>1.76895E-7</c:v>
+                </c:pt>
+                <c:pt idx="58" formatCode="0.00E+00">
+                  <c:v>1.38589E-7</c:v>
+                </c:pt>
+                <c:pt idx="59" formatCode="0.00E+00">
+                  <c:v>1.08445E-7</c:v>
+                </c:pt>
+                <c:pt idx="60" formatCode="0.00E+00">
+                  <c:v>8.53873E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Convergence Study'!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Direct 5 Point</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Convergence Study'!$C$18:$C$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Convergence Study'!$D$18:$D$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.352</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1568</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.10752</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.075264</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0550502</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0379331</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0291963</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0202955</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0155405</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0113242</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.00834911</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0063211</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.00482491</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.00355816</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.00278803</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.00205815</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.00161102</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.00120106</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.000932441</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.000708896</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.000541042</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.000418475</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.000323771</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.00024727</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.00019431</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.000147695</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.000116574</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="0.00E+00">
+                  <c:v>8.86582E-5</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="0.00E+00">
+                  <c:v>6.99528E-5</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="0.00E+00">
+                  <c:v>5.34998E-5</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0.00E+00">
+                  <c:v>4.20022E-5</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0.00E+00">
+                  <c:v>3.24569E-5</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0.00E+00">
+                  <c:v>2.52414E-5</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0.00E+00">
+                  <c:v>1.96906E-5</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="0.00E+00">
+                  <c:v>1.53306E-5</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="0.00E+00">
+                  <c:v>1.19488E-5</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="0.00E+00">
+                  <c:v>9.38751E-6</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="0.00E+00">
+                  <c:v>7.25412E-6</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="0.00E+00">
+                  <c:v>5.74662E-6</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="0.00E+00">
+                  <c:v>4.43824E-6</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="0.00E+00">
+                  <c:v>3.51759E-6</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="0.00E+00">
+                  <c:v>2.71746E-6</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="0.00E+00">
+                  <c:v>2.15339E-6</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="0.00E+00">
+                  <c:v>1.66687E-6</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="0.00E+00">
+                  <c:v>1.31857E-6</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="0.00E+00">
+                  <c:v>1.02704E-6</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="0.00E+00">
+                  <c:v>8.07668E-7</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="0.00E+00">
+                  <c:v>6.3278E-7</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="0.00E+00">
+                  <c:v>4.94928E-7</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="0.00E+00">
+                  <c:v>3.89889E-7</c:v>
+                </c:pt>
+                <c:pt idx="54" formatCode="0.00E+00">
+                  <c:v>3.06438E-7</c:v>
+                </c:pt>
+                <c:pt idx="55" formatCode="0.00E+00">
+                  <c:v>2.40266E-7</c:v>
+                </c:pt>
+                <c:pt idx="56" formatCode="0.00E+00">
+                  <c:v>1.8986E-7</c:v>
+                </c:pt>
+                <c:pt idx="57" formatCode="0.00E+00">
+                  <c:v>1.48094E-7</c:v>
+                </c:pt>
+                <c:pt idx="58" formatCode="0.00E+00">
+                  <c:v>1.17619E-7</c:v>
+                </c:pt>
+                <c:pt idx="59" formatCode="0.00E+00">
+                  <c:v>9.17018E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Convergence Study'!$E$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Adjoint 9 Point</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Convergence Study'!$E$18:$E$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Convergence Study'!$F$18:$F$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>4.23077</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.13641</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.62737</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.626271</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.371182</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.229985</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.139608</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.089023</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0562968</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0366427</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0248313</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0169751</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0116873</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.00807971</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0056183</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.00392453</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.00275495</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.00194223</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.00137504</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.000987301</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.000714682</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0005183</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.000376538</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.00027401</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.000199716</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.000145784</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.000106567</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0.00E+00">
+                  <c:v>7.8003E-5</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="0.00E+00">
+                  <c:v>5.71667E-5</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="0.00E+00">
+                  <c:v>4.19454E-5</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="0.00E+00">
+                  <c:v>3.09051E-5</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="0.00E+00">
+                  <c:v>2.2882E-5</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="0.00E+00">
+                  <c:v>1.69499E-5</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="0.00E+00">
+                  <c:v>1.25615E-5</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0.00E+00">
+                  <c:v>9.31364E-6</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0.00E+00">
+                  <c:v>6.90865E-6</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0.00E+00">
+                  <c:v>5.12708E-6</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0.00E+00">
+                  <c:v>3.80618E-6</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="0.00E+00">
+                  <c:v>2.82671E-6</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="0.00E+00">
+                  <c:v>2.10034E-6</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="0.00E+00">
+                  <c:v>1.56146E-6</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="0.00E+00">
+                  <c:v>1.16103E-6</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="0.00E+00">
+                  <c:v>8.63466E-7</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="0.00E+00">
+                  <c:v>6.4247E-7</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="0.00E+00">
+                  <c:v>4.78294E-7</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="0.00E+00">
+                  <c:v>3.56062E-7</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="0.00E+00">
+                  <c:v>2.65181E-7</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="0.00E+00">
+                  <c:v>1.97778E-7</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="0.00E+00">
+                  <c:v>1.47867E-7</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="0.00E+00">
+                  <c:v>1.10543E-7</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="0.00E+00">
+                  <c:v>8.26898E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Convergence Study'!$G$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Direct 9 Point</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Convergence Study'!$G$18:$G$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Convergence Study'!$H$18:$H$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>4.23077</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.09467</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.582613</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.328682</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.198226</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.122722</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0819781</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0562759</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0386816</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0265797</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0183421</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0127734</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.00904921</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.00654982</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0047389</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.00342732</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.00247924</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.00179433</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.00129963</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.000942186</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.000690367</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.000507643</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.000375779</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.000278086</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.000205765</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.000152253</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.000112671</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0.00E+00">
+                  <c:v>8.3396E-5</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="0.00E+00">
+                  <c:v>6.17435E-5</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="0.00E+00">
+                  <c:v>4.57271E-5</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="0.00E+00">
+                  <c:v>3.39877E-5</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="0.00E+00">
+                  <c:v>2.53193E-5</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="0.00E+00">
+                  <c:v>1.89221E-5</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="0.00E+00">
+                  <c:v>1.41737E-5</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0.00E+00">
+                  <c:v>1.06157E-5</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0.00E+00">
+                  <c:v>7.95043E-6</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0.00E+00">
+                  <c:v>5.95427E-6</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0.00E+00">
+                  <c:v>4.45941E-6</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="0.00E+00">
+                  <c:v>3.34005E-6</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="0.00E+00">
+                  <c:v>2.50187E-6</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="0.00E+00">
+                  <c:v>1.87424E-6</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="0.00E+00">
+                  <c:v>1.40424E-6</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="0.00E+00">
+                  <c:v>1.05258E-6</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="0.00E+00">
+                  <c:v>7.91413E-7</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="0.00E+00">
+                  <c:v>5.95068E-7</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="0.00E+00">
+                  <c:v>4.48479E-7</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="0.00E+00">
+                  <c:v>3.3833E-7</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="0.00E+00">
+                  <c:v>2.55222E-7</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="0.00E+00">
+                  <c:v>1.92524E-7</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="0.00E+00">
+                  <c:v>1.45226E-7</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="0.00E+00">
+                  <c:v>1.09549E-7</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="0.00E+00">
+                  <c:v>8.2638E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2123903096"/>
+        <c:axId val="2123642888"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2123903096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="61.0"/>
+          <c:min val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iteration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2123642888"/>
+        <c:crossesAt val="1.0E-8"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2123642888"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Residual Inf_Norm</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.00722543352601156"/>
+              <c:y val="0.430642711231535"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2123903096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -976,12 +2870,12 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:colOff>533400</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
@@ -1027,6 +2921,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1359,8 +3288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1684,6 +3613,1641 @@
       </c>
       <c r="K21">
         <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1E-8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>4.2307699999999997</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>4.2307699999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>3.0655000000000001</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1.2</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>4.1364099999999997</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>1.09467</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>1.5100800000000001</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>0.64</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>1.62737</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>0.58261300000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>0.827511</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>0.62627100000000002</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <v>0.32868199999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>0.45778999999999997</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>0.37118200000000001</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>0.19822600000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>0.32209500000000002</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>0.15679999999999999</v>
+      </c>
+      <c r="E23">
+        <v>6</v>
+      </c>
+      <c r="F23">
+        <v>0.22998499999999999</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <v>0.122722</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>0.191576</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>0.10752</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>0.13960800000000001</v>
+      </c>
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>8.1978099999999998E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>0.13731199999999999</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>7.5263999999999998E-2</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25">
+        <v>8.9023000000000005E-2</v>
+      </c>
+      <c r="G25">
+        <v>8</v>
+      </c>
+      <c r="H25">
+        <v>5.6275899999999997E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>9.1996599999999998E-2</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>5.5050200000000001E-2</v>
+      </c>
+      <c r="E26">
+        <v>9</v>
+      </c>
+      <c r="F26">
+        <v>5.6296800000000001E-2</v>
+      </c>
+      <c r="G26">
+        <v>9</v>
+      </c>
+      <c r="H26">
+        <v>3.8681599999999997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>6.32601E-2</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>3.7933099999999997E-2</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <v>3.66427E-2</v>
+      </c>
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>2.6579700000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <v>4.5238500000000001E-2</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>2.9196300000000001E-2</v>
+      </c>
+      <c r="E28">
+        <v>11</v>
+      </c>
+      <c r="F28">
+        <v>2.4831300000000001E-2</v>
+      </c>
+      <c r="G28">
+        <v>11</v>
+      </c>
+      <c r="H28">
+        <v>1.83421E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>12</v>
+      </c>
+      <c r="B29">
+        <v>3.2290300000000001E-2</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>2.0295500000000001E-2</v>
+      </c>
+      <c r="E29">
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>1.69751E-2</v>
+      </c>
+      <c r="G29">
+        <v>12</v>
+      </c>
+      <c r="H29">
+        <v>1.2773400000000001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>13</v>
+      </c>
+      <c r="B30">
+        <v>2.3428899999999999E-2</v>
+      </c>
+      <c r="C30">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>1.55405E-2</v>
+      </c>
+      <c r="E30">
+        <v>13</v>
+      </c>
+      <c r="F30">
+        <v>1.1687299999999999E-2</v>
+      </c>
+      <c r="G30">
+        <v>13</v>
+      </c>
+      <c r="H30">
+        <v>9.0492100000000002E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>1.73023E-2</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>1.13242E-2</v>
+      </c>
+      <c r="E31">
+        <v>14</v>
+      </c>
+      <c r="F31">
+        <v>8.0797100000000004E-3</v>
+      </c>
+      <c r="G31">
+        <v>14</v>
+      </c>
+      <c r="H31">
+        <v>6.5498199999999996E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <v>1.25367E-2</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>8.3491099999999999E-3</v>
+      </c>
+      <c r="E32">
+        <v>15</v>
+      </c>
+      <c r="F32">
+        <v>5.6182999999999997E-3</v>
+      </c>
+      <c r="G32">
+        <v>15</v>
+      </c>
+      <c r="H32">
+        <v>4.7388999999999999E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>9.3289900000000005E-3</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>6.3210999999999996E-3</v>
+      </c>
+      <c r="E33">
+        <v>16</v>
+      </c>
+      <c r="F33">
+        <v>3.9245299999999999E-3</v>
+      </c>
+      <c r="G33">
+        <v>16</v>
+      </c>
+      <c r="H33">
+        <v>3.4273200000000002E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>6.7580699999999997E-3</v>
+      </c>
+      <c r="C34">
+        <v>17</v>
+      </c>
+      <c r="D34">
+        <v>4.82491E-3</v>
+      </c>
+      <c r="E34">
+        <v>17</v>
+      </c>
+      <c r="F34">
+        <v>2.7549499999999999E-3</v>
+      </c>
+      <c r="G34">
+        <v>17</v>
+      </c>
+      <c r="H34">
+        <v>2.4792400000000002E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>5.0667999999999998E-3</v>
+      </c>
+      <c r="C35">
+        <v>18</v>
+      </c>
+      <c r="D35">
+        <v>3.5581599999999999E-3</v>
+      </c>
+      <c r="E35">
+        <v>18</v>
+      </c>
+      <c r="F35">
+        <v>1.9422300000000001E-3</v>
+      </c>
+      <c r="G35">
+        <v>18</v>
+      </c>
+      <c r="H35">
+        <v>1.79433E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <v>3.6701199999999998E-3</v>
+      </c>
+      <c r="C36">
+        <v>19</v>
+      </c>
+      <c r="D36">
+        <v>2.7880299999999999E-3</v>
+      </c>
+      <c r="E36">
+        <v>19</v>
+      </c>
+      <c r="F36">
+        <v>1.3750399999999999E-3</v>
+      </c>
+      <c r="G36">
+        <v>19</v>
+      </c>
+      <c r="H36">
+        <v>1.29963E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37">
+        <v>20</v>
+      </c>
+      <c r="B37">
+        <v>2.7727400000000001E-3</v>
+      </c>
+      <c r="C37">
+        <v>20</v>
+      </c>
+      <c r="D37">
+        <v>2.0581499999999999E-3</v>
+      </c>
+      <c r="E37">
+        <v>20</v>
+      </c>
+      <c r="F37">
+        <v>9.8730100000000011E-4</v>
+      </c>
+      <c r="G37">
+        <v>20</v>
+      </c>
+      <c r="H37">
+        <v>9.4218600000000002E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <v>2.0073299999999999E-3</v>
+      </c>
+      <c r="C38">
+        <v>21</v>
+      </c>
+      <c r="D38">
+        <v>1.6110199999999999E-3</v>
+      </c>
+      <c r="E38">
+        <v>21</v>
+      </c>
+      <c r="F38">
+        <v>7.1468200000000001E-4</v>
+      </c>
+      <c r="G38">
+        <v>21</v>
+      </c>
+      <c r="H38">
+        <v>6.90367E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39">
+        <v>22</v>
+      </c>
+      <c r="B39">
+        <v>1.5676799999999999E-3</v>
+      </c>
+      <c r="C39">
+        <v>22</v>
+      </c>
+      <c r="D39">
+        <v>1.2010600000000001E-3</v>
+      </c>
+      <c r="E39">
+        <v>22</v>
+      </c>
+      <c r="F39">
+        <v>5.1829999999999997E-4</v>
+      </c>
+      <c r="G39">
+        <v>22</v>
+      </c>
+      <c r="H39">
+        <v>5.07643E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40">
+        <v>23</v>
+      </c>
+      <c r="B40">
+        <v>1.1850700000000001E-3</v>
+      </c>
+      <c r="C40">
+        <v>23</v>
+      </c>
+      <c r="D40">
+        <v>9.32441E-4</v>
+      </c>
+      <c r="E40">
+        <v>23</v>
+      </c>
+      <c r="F40">
+        <v>3.7653799999999999E-4</v>
+      </c>
+      <c r="G40">
+        <v>23</v>
+      </c>
+      <c r="H40">
+        <v>3.7577900000000002E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41">
+        <v>24</v>
+      </c>
+      <c r="B41">
+        <v>9.2259700000000004E-4</v>
+      </c>
+      <c r="C41">
+        <v>24</v>
+      </c>
+      <c r="D41">
+        <v>7.0889599999999998E-4</v>
+      </c>
+      <c r="E41">
+        <v>24</v>
+      </c>
+      <c r="F41">
+        <v>2.7400999999999999E-4</v>
+      </c>
+      <c r="G41">
+        <v>24</v>
+      </c>
+      <c r="H41">
+        <v>2.7808599999999998E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42">
+        <v>25</v>
+      </c>
+      <c r="B42">
+        <v>7.0223400000000004E-4</v>
+      </c>
+      <c r="C42">
+        <v>25</v>
+      </c>
+      <c r="D42">
+        <v>5.4104200000000004E-4</v>
+      </c>
+      <c r="E42">
+        <v>25</v>
+      </c>
+      <c r="F42">
+        <v>1.9971600000000001E-4</v>
+      </c>
+      <c r="G42">
+        <v>25</v>
+      </c>
+      <c r="H42">
+        <v>2.0576500000000001E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43">
+        <v>26</v>
+      </c>
+      <c r="B43">
+        <v>5.4324400000000002E-4</v>
+      </c>
+      <c r="C43">
+        <v>26</v>
+      </c>
+      <c r="D43">
+        <v>4.1847500000000002E-4</v>
+      </c>
+      <c r="E43">
+        <v>26</v>
+      </c>
+      <c r="F43">
+        <v>1.4578400000000001E-4</v>
+      </c>
+      <c r="G43">
+        <v>26</v>
+      </c>
+      <c r="H43">
+        <v>1.5225300000000001E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44">
+        <v>27</v>
+      </c>
+      <c r="B44">
+        <v>4.1631300000000002E-4</v>
+      </c>
+      <c r="C44">
+        <v>27</v>
+      </c>
+      <c r="D44">
+        <v>3.2377099999999999E-4</v>
+      </c>
+      <c r="E44">
+        <v>27</v>
+      </c>
+      <c r="F44">
+        <v>1.06567E-4</v>
+      </c>
+      <c r="G44">
+        <v>27</v>
+      </c>
+      <c r="H44">
+        <v>1.1267100000000001E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45">
+        <v>28</v>
+      </c>
+      <c r="B45">
+        <v>3.2022000000000002E-4</v>
+      </c>
+      <c r="C45">
+        <v>28</v>
+      </c>
+      <c r="D45">
+        <v>2.4727000000000001E-4</v>
+      </c>
+      <c r="E45">
+        <v>28</v>
+      </c>
+      <c r="F45" s="2">
+        <v>7.8003000000000005E-5</v>
+      </c>
+      <c r="G45">
+        <v>28</v>
+      </c>
+      <c r="H45" s="2">
+        <v>8.3395999999999999E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46">
+        <v>29</v>
+      </c>
+      <c r="B46">
+        <v>2.4830300000000001E-4</v>
+      </c>
+      <c r="C46">
+        <v>29</v>
+      </c>
+      <c r="D46">
+        <v>1.9431E-4</v>
+      </c>
+      <c r="E46">
+        <v>29</v>
+      </c>
+      <c r="F46" s="2">
+        <v>5.7166700000000003E-5</v>
+      </c>
+      <c r="G46">
+        <v>29</v>
+      </c>
+      <c r="H46" s="2">
+        <v>6.1743500000000003E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47">
+        <v>30</v>
+      </c>
+      <c r="B47">
+        <v>1.9066800000000001E-4</v>
+      </c>
+      <c r="C47">
+        <v>30</v>
+      </c>
+      <c r="D47">
+        <v>1.4769499999999999E-4</v>
+      </c>
+      <c r="E47">
+        <v>30</v>
+      </c>
+      <c r="F47" s="2">
+        <v>4.19454E-5</v>
+      </c>
+      <c r="G47">
+        <v>30</v>
+      </c>
+      <c r="H47" s="2">
+        <v>4.5727099999999998E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48">
+        <v>31</v>
+      </c>
+      <c r="B48">
+        <v>1.48665E-4</v>
+      </c>
+      <c r="C48">
+        <v>31</v>
+      </c>
+      <c r="D48">
+        <v>1.16574E-4</v>
+      </c>
+      <c r="E48">
+        <v>31</v>
+      </c>
+      <c r="F48" s="2">
+        <v>3.0905100000000003E-5</v>
+      </c>
+      <c r="G48">
+        <v>31</v>
+      </c>
+      <c r="H48" s="2">
+        <v>3.39877E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>32</v>
+      </c>
+      <c r="B49">
+        <v>1.1501399999999999E-4</v>
+      </c>
+      <c r="C49">
+        <v>32</v>
+      </c>
+      <c r="D49" s="2">
+        <v>8.8658200000000004E-5</v>
+      </c>
+      <c r="E49">
+        <v>32</v>
+      </c>
+      <c r="F49" s="2">
+        <v>2.2881999999999999E-5</v>
+      </c>
+      <c r="G49">
+        <v>32</v>
+      </c>
+      <c r="H49" s="2">
+        <v>2.53193E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50">
+        <v>33</v>
+      </c>
+      <c r="B50" s="2">
+        <v>8.9018999999999996E-5</v>
+      </c>
+      <c r="C50">
+        <v>33</v>
+      </c>
+      <c r="D50" s="2">
+        <v>6.9952799999999999E-5</v>
+      </c>
+      <c r="E50">
+        <v>33</v>
+      </c>
+      <c r="F50" s="2">
+        <v>1.6949899999999998E-5</v>
+      </c>
+      <c r="G50">
+        <v>33</v>
+      </c>
+      <c r="H50" s="2">
+        <v>1.89221E-5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51">
+        <v>34</v>
+      </c>
+      <c r="B51" s="2">
+        <v>6.9352300000000003E-5</v>
+      </c>
+      <c r="C51">
+        <v>34</v>
+      </c>
+      <c r="D51" s="2">
+        <v>5.3499799999999999E-5</v>
+      </c>
+      <c r="E51">
+        <v>34</v>
+      </c>
+      <c r="F51" s="2">
+        <v>1.25615E-5</v>
+      </c>
+      <c r="G51">
+        <v>34</v>
+      </c>
+      <c r="H51" s="2">
+        <v>1.4173699999999999E-5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52">
+        <v>35</v>
+      </c>
+      <c r="B52" s="2">
+        <v>5.3328500000000003E-5</v>
+      </c>
+      <c r="C52">
+        <v>35</v>
+      </c>
+      <c r="D52" s="2">
+        <v>4.2002200000000002E-5</v>
+      </c>
+      <c r="E52">
+        <v>35</v>
+      </c>
+      <c r="F52" s="2">
+        <v>9.3136399999999995E-6</v>
+      </c>
+      <c r="G52">
+        <v>35</v>
+      </c>
+      <c r="H52" s="2">
+        <v>1.0615700000000001E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53">
+        <v>36</v>
+      </c>
+      <c r="B53" s="2">
+        <v>4.1819600000000002E-5</v>
+      </c>
+      <c r="C53">
+        <v>36</v>
+      </c>
+      <c r="D53" s="2">
+        <v>3.2456899999999998E-5</v>
+      </c>
+      <c r="E53">
+        <v>36</v>
+      </c>
+      <c r="F53" s="2">
+        <v>6.9086500000000003E-6</v>
+      </c>
+      <c r="G53">
+        <v>36</v>
+      </c>
+      <c r="H53" s="2">
+        <v>7.9504299999999997E-6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54">
+        <v>37</v>
+      </c>
+      <c r="B54" s="2">
+        <v>3.19699E-5</v>
+      </c>
+      <c r="C54">
+        <v>37</v>
+      </c>
+      <c r="D54" s="2">
+        <v>2.5241399999999999E-5</v>
+      </c>
+      <c r="E54">
+        <v>37</v>
+      </c>
+      <c r="F54" s="2">
+        <v>5.1270799999999999E-6</v>
+      </c>
+      <c r="G54">
+        <v>37</v>
+      </c>
+      <c r="H54" s="2">
+        <v>5.9542700000000003E-6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55">
+        <v>38</v>
+      </c>
+      <c r="B55" s="2">
+        <v>2.5224699999999999E-5</v>
+      </c>
+      <c r="C55">
+        <v>38</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1.9690600000000001E-5</v>
+      </c>
+      <c r="E55">
+        <v>38</v>
+      </c>
+      <c r="F55" s="2">
+        <v>3.80618E-6</v>
+      </c>
+      <c r="G55">
+        <v>38</v>
+      </c>
+      <c r="H55" s="2">
+        <v>4.4594099999999999E-6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56">
+        <v>39</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1.9325800000000001E-5</v>
+      </c>
+      <c r="C56">
+        <v>39</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1.5330599999999999E-5</v>
+      </c>
+      <c r="E56">
+        <v>39</v>
+      </c>
+      <c r="F56" s="2">
+        <v>2.8267099999999998E-6</v>
+      </c>
+      <c r="G56">
+        <v>39</v>
+      </c>
+      <c r="H56" s="2">
+        <v>3.3400499999999999E-6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57">
+        <v>40</v>
+      </c>
+      <c r="B57" s="2">
+        <v>1.52225E-5</v>
+      </c>
+      <c r="C57">
+        <v>40</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1.19488E-5</v>
+      </c>
+      <c r="E57">
+        <v>40</v>
+      </c>
+      <c r="F57" s="2">
+        <v>2.1003399999999999E-6</v>
+      </c>
+      <c r="G57">
+        <v>40</v>
+      </c>
+      <c r="H57" s="2">
+        <v>2.5018700000000002E-6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58">
+        <v>41</v>
+      </c>
+      <c r="B58" s="2">
+        <v>1.17774E-5</v>
+      </c>
+      <c r="C58">
+        <v>41</v>
+      </c>
+      <c r="D58" s="2">
+        <v>9.3875100000000002E-6</v>
+      </c>
+      <c r="E58">
+        <v>41</v>
+      </c>
+      <c r="F58" s="2">
+        <v>1.56146E-6</v>
+      </c>
+      <c r="G58">
+        <v>41</v>
+      </c>
+      <c r="H58" s="2">
+        <v>1.87424E-6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59">
+        <v>42</v>
+      </c>
+      <c r="B59" s="2">
+        <v>9.1921400000000007E-6</v>
+      </c>
+      <c r="C59">
+        <v>42</v>
+      </c>
+      <c r="D59" s="2">
+        <v>7.2541200000000003E-6</v>
+      </c>
+      <c r="E59">
+        <v>42</v>
+      </c>
+      <c r="F59" s="2">
+        <v>1.16103E-6</v>
+      </c>
+      <c r="G59">
+        <v>42</v>
+      </c>
+      <c r="H59" s="2">
+        <v>1.4042400000000001E-6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60">
+        <v>43</v>
+      </c>
+      <c r="B60" s="2">
+        <v>7.1757700000000004E-6</v>
+      </c>
+      <c r="C60">
+        <v>43</v>
+      </c>
+      <c r="D60" s="2">
+        <v>5.7466199999999999E-6</v>
+      </c>
+      <c r="E60">
+        <v>43</v>
+      </c>
+      <c r="F60" s="2">
+        <v>8.6346599999999998E-7</v>
+      </c>
+      <c r="G60">
+        <v>43</v>
+      </c>
+      <c r="H60" s="2">
+        <v>1.05258E-6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61">
+        <v>44</v>
+      </c>
+      <c r="B61" s="2">
+        <v>5.5547100000000002E-6</v>
+      </c>
+      <c r="C61">
+        <v>44</v>
+      </c>
+      <c r="D61" s="2">
+        <v>4.4382400000000004E-6</v>
+      </c>
+      <c r="E61">
+        <v>44</v>
+      </c>
+      <c r="F61" s="2">
+        <v>6.4247000000000001E-7</v>
+      </c>
+      <c r="G61">
+        <v>44</v>
+      </c>
+      <c r="H61" s="2">
+        <v>7.9141299999999999E-7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62">
+        <v>45</v>
+      </c>
+      <c r="B62" s="2">
+        <v>4.3719800000000001E-6</v>
+      </c>
+      <c r="C62">
+        <v>45</v>
+      </c>
+      <c r="D62" s="2">
+        <v>3.5175900000000001E-6</v>
+      </c>
+      <c r="E62">
+        <v>45</v>
+      </c>
+      <c r="F62" s="2">
+        <v>4.7829399999999998E-7</v>
+      </c>
+      <c r="G62">
+        <v>45</v>
+      </c>
+      <c r="H62" s="2">
+        <v>5.9506799999999999E-7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63">
+        <v>46</v>
+      </c>
+      <c r="B63" s="2">
+        <v>3.3592700000000002E-6</v>
+      </c>
+      <c r="C63">
+        <v>46</v>
+      </c>
+      <c r="D63" s="2">
+        <v>2.71746E-6</v>
+      </c>
+      <c r="E63">
+        <v>46</v>
+      </c>
+      <c r="F63" s="2">
+        <v>3.5606199999999998E-7</v>
+      </c>
+      <c r="G63">
+        <v>46</v>
+      </c>
+      <c r="H63" s="2">
+        <v>4.4847899999999998E-7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64">
+        <v>47</v>
+      </c>
+      <c r="B64" s="2">
+        <v>2.6640600000000002E-6</v>
+      </c>
+      <c r="C64">
+        <v>47</v>
+      </c>
+      <c r="D64" s="2">
+        <v>2.1533900000000001E-6</v>
+      </c>
+      <c r="E64">
+        <v>47</v>
+      </c>
+      <c r="F64" s="2">
+        <v>2.6518100000000002E-7</v>
+      </c>
+      <c r="G64">
+        <v>47</v>
+      </c>
+      <c r="H64" s="2">
+        <v>3.3832999999999999E-7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65">
+        <v>48</v>
+      </c>
+      <c r="B65" s="2">
+        <v>2.05042E-6</v>
+      </c>
+      <c r="C65">
+        <v>48</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1.6668700000000001E-6</v>
+      </c>
+      <c r="E65">
+        <v>48</v>
+      </c>
+      <c r="F65" s="2">
+        <v>1.9777800000000001E-7</v>
+      </c>
+      <c r="G65">
+        <v>48</v>
+      </c>
+      <c r="H65" s="2">
+        <v>2.5522199999999998E-7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66">
+        <v>49</v>
+      </c>
+      <c r="B66" s="2">
+        <v>1.62373E-6</v>
+      </c>
+      <c r="C66">
+        <v>49</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1.31857E-6</v>
+      </c>
+      <c r="E66">
+        <v>49</v>
+      </c>
+      <c r="F66" s="2">
+        <v>1.4786700000000001E-7</v>
+      </c>
+      <c r="G66">
+        <v>49</v>
+      </c>
+      <c r="H66" s="2">
+        <v>1.9252400000000001E-7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67">
+        <v>50</v>
+      </c>
+      <c r="B67" s="2">
+        <v>1.2556999999999999E-6</v>
+      </c>
+      <c r="C67">
+        <v>50</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1.0270399999999999E-6</v>
+      </c>
+      <c r="E67">
+        <v>50</v>
+      </c>
+      <c r="F67" s="2">
+        <v>1.10543E-7</v>
+      </c>
+      <c r="G67">
+        <v>50</v>
+      </c>
+      <c r="H67" s="2">
+        <v>1.4522600000000001E-7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68">
+        <v>51</v>
+      </c>
+      <c r="B68" s="2">
+        <v>9.8997299999999994E-7</v>
+      </c>
+      <c r="C68">
+        <v>51</v>
+      </c>
+      <c r="D68" s="2">
+        <v>8.0766799999999998E-7</v>
+      </c>
+      <c r="E68">
+        <v>51</v>
+      </c>
+      <c r="F68" s="2">
+        <v>8.2689799999999997E-8</v>
+      </c>
+      <c r="G68">
+        <v>51</v>
+      </c>
+      <c r="H68" s="2">
+        <v>1.09549E-7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69">
+        <v>52</v>
+      </c>
+      <c r="B69" s="2">
+        <v>7.6906499999999996E-7</v>
+      </c>
+      <c r="C69">
+        <v>52</v>
+      </c>
+      <c r="D69" s="2">
+        <v>6.3277999999999998E-7</v>
+      </c>
+      <c r="G69">
+        <v>52</v>
+      </c>
+      <c r="H69" s="2">
+        <v>8.2638000000000002E-8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70">
+        <v>53</v>
+      </c>
+      <c r="B70" s="2">
+        <v>6.0381199999999995E-7</v>
+      </c>
+      <c r="C70">
+        <v>53</v>
+      </c>
+      <c r="D70" s="2">
+        <v>4.9492800000000005E-7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71">
+        <v>54</v>
+      </c>
+      <c r="B71" s="2">
+        <v>4.7109600000000003E-7</v>
+      </c>
+      <c r="C71">
+        <v>54</v>
+      </c>
+      <c r="D71" s="2">
+        <v>3.8988899999999998E-7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72">
+        <v>55</v>
+      </c>
+      <c r="B72" s="2">
+        <v>3.6844199999999998E-7</v>
+      </c>
+      <c r="C72">
+        <v>55</v>
+      </c>
+      <c r="D72" s="2">
+        <v>3.0643799999999998E-7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73">
+        <v>56</v>
+      </c>
+      <c r="B73" s="2">
+        <v>2.8863800000000002E-7</v>
+      </c>
+      <c r="C73">
+        <v>56</v>
+      </c>
+      <c r="D73" s="2">
+        <v>2.4026600000000002E-7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74">
+        <v>57</v>
+      </c>
+      <c r="B74" s="2">
+        <v>2.2492999999999999E-7</v>
+      </c>
+      <c r="C74">
+        <v>57</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1.8986000000000001E-7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75">
+        <v>58</v>
+      </c>
+      <c r="B75" s="2">
+        <v>1.76895E-7</v>
+      </c>
+      <c r="C75">
+        <v>58</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1.48094E-7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76">
+        <v>59</v>
+      </c>
+      <c r="B76" s="2">
+        <v>1.38589E-7</v>
+      </c>
+      <c r="C76">
+        <v>59</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1.17619E-7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77">
+        <v>60</v>
+      </c>
+      <c r="B77" s="2">
+        <v>1.08445E-7</v>
+      </c>
+      <c r="C77">
+        <v>60</v>
+      </c>
+      <c r="D77" s="2">
+        <v>9.1701799999999999E-8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78">
+        <v>61</v>
+      </c>
+      <c r="B78" s="2">
+        <v>8.5387299999999999E-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding adjoint vs. direct convergence data and figures
</commit_message>
<xml_diff>
--- a/doc/hmcsa_adjoint_vs_direct/direct_vs_adjoint.xlsx
+++ b/doc/hmcsa_adjoint_vs_direct/direct_vs_adjoint.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="0" windowWidth="25820" windowHeight="23480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7180" yWindow="0" windowWidth="26400" windowHeight="20480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Timing Study" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>problem parameters</t>
   </si>
@@ -154,8 +154,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -182,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -192,6 +206,13 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -201,6 +222,13 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -600,11 +628,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121052280"/>
-        <c:axId val="2121057976"/>
+        <c:axId val="2050134968"/>
+        <c:axId val="2050209320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121052280"/>
+        <c:axId val="2050134968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="101.0"/>
@@ -639,12 +667,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121057976"/>
+        <c:crossAx val="2050209320"/>
         <c:crossesAt val="0.01"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121057976"/>
+        <c:axId val="2050209320"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -675,7 +703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121052280"/>
+        <c:crossAx val="2050134968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1093,11 +1121,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121099768"/>
-        <c:axId val="2121105576"/>
+        <c:axId val="2076809560"/>
+        <c:axId val="2076815352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121099768"/>
+        <c:axId val="2076809560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="101.0"/>
@@ -1133,12 +1161,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121105576"/>
+        <c:crossAx val="2076815352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121105576"/>
+        <c:axId val="2076815352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40.0"/>
@@ -1169,7 +1197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121099768"/>
+        <c:crossAx val="2076809560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1239,7 +1267,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Convergence Study'!$A$16</c:f>
+              <c:f>'Convergence Study'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1649,11 +1677,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Convergence Study'!$C$16</c:f>
+              <c:f>'Convergence Study'!#REF!</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Direct 5 Point</c:v>
+                  <c:v>#REF!</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1670,196 +1698,12 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Convergence Study'!$C$18:$C$77</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>60.0</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>'Convergence Study'!#REF!</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Convergence Study'!$D$18:$D$77</c:f>
+              <c:f>'Convergence Study'!$C$18:$C$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -2053,7 +1897,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Convergence Study'!$E$16</c:f>
+              <c:f>'Convergence Study'!$D$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2074,169 +1918,12 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Convergence Study'!$E$18:$E$68</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="51"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>51.0</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>'Convergence Study'!#REF!</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Convergence Study'!$F$18:$F$68</c:f>
+              <c:f>'Convergence Study'!$D$18:$D$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2403,7 +2090,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Convergence Study'!$G$16</c:f>
+              <c:f>'Convergence Study'!$E$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2426,172 +2113,12 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Convergence Study'!$G$18:$G$69</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>52.0</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>'Convergence Study'!#REF!</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Convergence Study'!$H$18:$H$69</c:f>
+              <c:f>'Convergence Study'!$E$18:$E$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
@@ -2764,11 +2291,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123903096"/>
-        <c:axId val="2123642888"/>
+        <c:axId val="2051518216"/>
+        <c:axId val="2051523688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123903096"/>
+        <c:axId val="2051518216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="61.0"/>
@@ -2799,12 +2326,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123642888"/>
+        <c:crossAx val="2051523688"/>
         <c:crossesAt val="1.0E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123642888"/>
+        <c:axId val="2051523688"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2842,7 +2369,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123903096"/>
+        <c:crossAx val="2051518216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2933,13 +2460,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>177800</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>711200</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -3288,8 +2815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView showRuler="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3629,42 +3156,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3672,7 +3202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3680,7 +3210,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3688,7 +3218,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3696,7 +3226,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3704,7 +3234,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3712,7 +3242,7 @@
         <v>1E-8</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3720,7 +3250,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3728,7 +3258,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -3736,7 +3266,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3744,21 +3274,21 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:5">
+      <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3766,25 +3296,16 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" t="s">
         <v>25</v>
       </c>
-      <c r="G17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3792,25 +3313,16 @@
         <v>4</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>4.2307699999999997</v>
       </c>
       <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
         <v>4.2307699999999997</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>4.2307699999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3818,25 +3330,16 @@
         <v>3.0655000000000001</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="D19">
-        <v>1.2</v>
+        <v>4.1364099999999997</v>
       </c>
       <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="F19">
-        <v>4.1364099999999997</v>
-      </c>
-      <c r="G19">
-        <v>2</v>
-      </c>
-      <c r="H19">
         <v>1.09467</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>3</v>
       </c>
@@ -3844,25 +3347,16 @@
         <v>1.5100800000000001</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>0.64</v>
       </c>
       <c r="D20">
-        <v>0.64</v>
+        <v>1.62737</v>
       </c>
       <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <v>1.62737</v>
-      </c>
-      <c r="G20">
-        <v>3</v>
-      </c>
-      <c r="H20">
         <v>0.58261300000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>4</v>
       </c>
@@ -3870,25 +3364,16 @@
         <v>0.827511</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="D21">
-        <v>0.35199999999999998</v>
+        <v>0.62627100000000002</v>
       </c>
       <c r="E21">
-        <v>4</v>
-      </c>
-      <c r="F21">
-        <v>0.62627100000000002</v>
-      </c>
-      <c r="G21">
-        <v>4</v>
-      </c>
-      <c r="H21">
         <v>0.32868199999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>5</v>
       </c>
@@ -3896,25 +3381,16 @@
         <v>0.45778999999999997</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="D22">
-        <v>0.25600000000000001</v>
+        <v>0.37118200000000001</v>
       </c>
       <c r="E22">
-        <v>5</v>
-      </c>
-      <c r="F22">
-        <v>0.37118200000000001</v>
-      </c>
-      <c r="G22">
-        <v>5</v>
-      </c>
-      <c r="H22">
         <v>0.19822600000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>6</v>
       </c>
@@ -3922,25 +3398,16 @@
         <v>0.32209500000000002</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>0.15679999999999999</v>
       </c>
       <c r="D23">
-        <v>0.15679999999999999</v>
+        <v>0.22998499999999999</v>
       </c>
       <c r="E23">
-        <v>6</v>
-      </c>
-      <c r="F23">
-        <v>0.22998499999999999</v>
-      </c>
-      <c r="G23">
-        <v>6</v>
-      </c>
-      <c r="H23">
         <v>0.122722</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>7</v>
       </c>
@@ -3948,25 +3415,16 @@
         <v>0.191576</v>
       </c>
       <c r="C24">
-        <v>7</v>
+        <v>0.10752</v>
       </c>
       <c r="D24">
-        <v>0.10752</v>
+        <v>0.13960800000000001</v>
       </c>
       <c r="E24">
-        <v>7</v>
-      </c>
-      <c r="F24">
-        <v>0.13960800000000001</v>
-      </c>
-      <c r="G24">
-        <v>7</v>
-      </c>
-      <c r="H24">
         <v>8.1978099999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>8</v>
       </c>
@@ -3974,25 +3432,16 @@
         <v>0.13731199999999999</v>
       </c>
       <c r="C25">
-        <v>8</v>
+        <v>7.5263999999999998E-2</v>
       </c>
       <c r="D25">
-        <v>7.5263999999999998E-2</v>
+        <v>8.9023000000000005E-2</v>
       </c>
       <c r="E25">
-        <v>8</v>
-      </c>
-      <c r="F25">
-        <v>8.9023000000000005E-2</v>
-      </c>
-      <c r="G25">
-        <v>8</v>
-      </c>
-      <c r="H25">
         <v>5.6275899999999997E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>9</v>
       </c>
@@ -4000,25 +3449,16 @@
         <v>9.1996599999999998E-2</v>
       </c>
       <c r="C26">
-        <v>9</v>
+        <v>5.5050200000000001E-2</v>
       </c>
       <c r="D26">
-        <v>5.5050200000000001E-2</v>
+        <v>5.6296800000000001E-2</v>
       </c>
       <c r="E26">
-        <v>9</v>
-      </c>
-      <c r="F26">
-        <v>5.6296800000000001E-2</v>
-      </c>
-      <c r="G26">
-        <v>9</v>
-      </c>
-      <c r="H26">
         <v>3.8681599999999997E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>10</v>
       </c>
@@ -4026,25 +3466,16 @@
         <v>6.32601E-2</v>
       </c>
       <c r="C27">
-        <v>10</v>
+        <v>3.7933099999999997E-2</v>
       </c>
       <c r="D27">
-        <v>3.7933099999999997E-2</v>
+        <v>3.66427E-2</v>
       </c>
       <c r="E27">
-        <v>10</v>
-      </c>
-      <c r="F27">
-        <v>3.66427E-2</v>
-      </c>
-      <c r="G27">
-        <v>10</v>
-      </c>
-      <c r="H27">
         <v>2.6579700000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>11</v>
       </c>
@@ -4052,25 +3483,16 @@
         <v>4.5238500000000001E-2</v>
       </c>
       <c r="C28">
-        <v>11</v>
+        <v>2.9196300000000001E-2</v>
       </c>
       <c r="D28">
-        <v>2.9196300000000001E-2</v>
+        <v>2.4831300000000001E-2</v>
       </c>
       <c r="E28">
-        <v>11</v>
-      </c>
-      <c r="F28">
-        <v>2.4831300000000001E-2</v>
-      </c>
-      <c r="G28">
-        <v>11</v>
-      </c>
-      <c r="H28">
         <v>1.83421E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>12</v>
       </c>
@@ -4078,25 +3500,16 @@
         <v>3.2290300000000001E-2</v>
       </c>
       <c r="C29">
-        <v>12</v>
+        <v>2.0295500000000001E-2</v>
       </c>
       <c r="D29">
-        <v>2.0295500000000001E-2</v>
+        <v>1.69751E-2</v>
       </c>
       <c r="E29">
-        <v>12</v>
-      </c>
-      <c r="F29">
-        <v>1.69751E-2</v>
-      </c>
-      <c r="G29">
-        <v>12</v>
-      </c>
-      <c r="H29">
         <v>1.2773400000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>13</v>
       </c>
@@ -4104,25 +3517,16 @@
         <v>2.3428899999999999E-2</v>
       </c>
       <c r="C30">
-        <v>13</v>
+        <v>1.55405E-2</v>
       </c>
       <c r="D30">
-        <v>1.55405E-2</v>
+        <v>1.1687299999999999E-2</v>
       </c>
       <c r="E30">
-        <v>13</v>
-      </c>
-      <c r="F30">
-        <v>1.1687299999999999E-2</v>
-      </c>
-      <c r="G30">
-        <v>13</v>
-      </c>
-      <c r="H30">
         <v>9.0492100000000002E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>14</v>
       </c>
@@ -4130,25 +3534,16 @@
         <v>1.73023E-2</v>
       </c>
       <c r="C31">
-        <v>14</v>
+        <v>1.13242E-2</v>
       </c>
       <c r="D31">
-        <v>1.13242E-2</v>
+        <v>8.0797100000000004E-3</v>
       </c>
       <c r="E31">
-        <v>14</v>
-      </c>
-      <c r="F31">
-        <v>8.0797100000000004E-3</v>
-      </c>
-      <c r="G31">
-        <v>14</v>
-      </c>
-      <c r="H31">
         <v>6.5498199999999996E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>15</v>
       </c>
@@ -4156,25 +3551,16 @@
         <v>1.25367E-2</v>
       </c>
       <c r="C32">
-        <v>15</v>
+        <v>8.3491099999999999E-3</v>
       </c>
       <c r="D32">
-        <v>8.3491099999999999E-3</v>
+        <v>5.6182999999999997E-3</v>
       </c>
       <c r="E32">
-        <v>15</v>
-      </c>
-      <c r="F32">
-        <v>5.6182999999999997E-3</v>
-      </c>
-      <c r="G32">
-        <v>15</v>
-      </c>
-      <c r="H32">
         <v>4.7388999999999999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>16</v>
       </c>
@@ -4182,25 +3568,16 @@
         <v>9.3289900000000005E-3</v>
       </c>
       <c r="C33">
-        <v>16</v>
+        <v>6.3210999999999996E-3</v>
       </c>
       <c r="D33">
-        <v>6.3210999999999996E-3</v>
+        <v>3.9245299999999999E-3</v>
       </c>
       <c r="E33">
-        <v>16</v>
-      </c>
-      <c r="F33">
-        <v>3.9245299999999999E-3</v>
-      </c>
-      <c r="G33">
-        <v>16</v>
-      </c>
-      <c r="H33">
         <v>3.4273200000000002E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>17</v>
       </c>
@@ -4208,25 +3585,16 @@
         <v>6.7580699999999997E-3</v>
       </c>
       <c r="C34">
-        <v>17</v>
+        <v>4.82491E-3</v>
       </c>
       <c r="D34">
-        <v>4.82491E-3</v>
+        <v>2.7549499999999999E-3</v>
       </c>
       <c r="E34">
-        <v>17</v>
-      </c>
-      <c r="F34">
-        <v>2.7549499999999999E-3</v>
-      </c>
-      <c r="G34">
-        <v>17</v>
-      </c>
-      <c r="H34">
         <v>2.4792400000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>18</v>
       </c>
@@ -4234,25 +3602,16 @@
         <v>5.0667999999999998E-3</v>
       </c>
       <c r="C35">
-        <v>18</v>
+        <v>3.5581599999999999E-3</v>
       </c>
       <c r="D35">
-        <v>3.5581599999999999E-3</v>
+        <v>1.9422300000000001E-3</v>
       </c>
       <c r="E35">
-        <v>18</v>
-      </c>
-      <c r="F35">
-        <v>1.9422300000000001E-3</v>
-      </c>
-      <c r="G35">
-        <v>18</v>
-      </c>
-      <c r="H35">
         <v>1.79433E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>19</v>
       </c>
@@ -4260,25 +3619,16 @@
         <v>3.6701199999999998E-3</v>
       </c>
       <c r="C36">
-        <v>19</v>
+        <v>2.7880299999999999E-3</v>
       </c>
       <c r="D36">
-        <v>2.7880299999999999E-3</v>
+        <v>1.3750399999999999E-3</v>
       </c>
       <c r="E36">
-        <v>19</v>
-      </c>
-      <c r="F36">
-        <v>1.3750399999999999E-3</v>
-      </c>
-      <c r="G36">
-        <v>19</v>
-      </c>
-      <c r="H36">
         <v>1.29963E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>20</v>
       </c>
@@ -4286,25 +3636,16 @@
         <v>2.7727400000000001E-3</v>
       </c>
       <c r="C37">
-        <v>20</v>
+        <v>2.0581499999999999E-3</v>
       </c>
       <c r="D37">
-        <v>2.0581499999999999E-3</v>
+        <v>9.8730100000000011E-4</v>
       </c>
       <c r="E37">
-        <v>20</v>
-      </c>
-      <c r="F37">
-        <v>9.8730100000000011E-4</v>
-      </c>
-      <c r="G37">
-        <v>20</v>
-      </c>
-      <c r="H37">
         <v>9.4218600000000002E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>21</v>
       </c>
@@ -4312,25 +3653,16 @@
         <v>2.0073299999999999E-3</v>
       </c>
       <c r="C38">
-        <v>21</v>
+        <v>1.6110199999999999E-3</v>
       </c>
       <c r="D38">
-        <v>1.6110199999999999E-3</v>
+        <v>7.1468200000000001E-4</v>
       </c>
       <c r="E38">
-        <v>21</v>
-      </c>
-      <c r="F38">
-        <v>7.1468200000000001E-4</v>
-      </c>
-      <c r="G38">
-        <v>21</v>
-      </c>
-      <c r="H38">
         <v>6.90367E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>22</v>
       </c>
@@ -4338,25 +3670,16 @@
         <v>1.5676799999999999E-3</v>
       </c>
       <c r="C39">
-        <v>22</v>
+        <v>1.2010600000000001E-3</v>
       </c>
       <c r="D39">
-        <v>1.2010600000000001E-3</v>
+        <v>5.1829999999999997E-4</v>
       </c>
       <c r="E39">
-        <v>22</v>
-      </c>
-      <c r="F39">
-        <v>5.1829999999999997E-4</v>
-      </c>
-      <c r="G39">
-        <v>22</v>
-      </c>
-      <c r="H39">
         <v>5.07643E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>23</v>
       </c>
@@ -4364,25 +3687,16 @@
         <v>1.1850700000000001E-3</v>
       </c>
       <c r="C40">
-        <v>23</v>
+        <v>9.32441E-4</v>
       </c>
       <c r="D40">
-        <v>9.32441E-4</v>
+        <v>3.7653799999999999E-4</v>
       </c>
       <c r="E40">
-        <v>23</v>
-      </c>
-      <c r="F40">
-        <v>3.7653799999999999E-4</v>
-      </c>
-      <c r="G40">
-        <v>23</v>
-      </c>
-      <c r="H40">
         <v>3.7577900000000002E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>24</v>
       </c>
@@ -4390,25 +3704,16 @@
         <v>9.2259700000000004E-4</v>
       </c>
       <c r="C41">
-        <v>24</v>
+        <v>7.0889599999999998E-4</v>
       </c>
       <c r="D41">
-        <v>7.0889599999999998E-4</v>
+        <v>2.7400999999999999E-4</v>
       </c>
       <c r="E41">
-        <v>24</v>
-      </c>
-      <c r="F41">
-        <v>2.7400999999999999E-4</v>
-      </c>
-      <c r="G41">
-        <v>24</v>
-      </c>
-      <c r="H41">
         <v>2.7808599999999998E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>25</v>
       </c>
@@ -4416,25 +3721,16 @@
         <v>7.0223400000000004E-4</v>
       </c>
       <c r="C42">
-        <v>25</v>
+        <v>5.4104200000000004E-4</v>
       </c>
       <c r="D42">
-        <v>5.4104200000000004E-4</v>
+        <v>1.9971600000000001E-4</v>
       </c>
       <c r="E42">
-        <v>25</v>
-      </c>
-      <c r="F42">
-        <v>1.9971600000000001E-4</v>
-      </c>
-      <c r="G42">
-        <v>25</v>
-      </c>
-      <c r="H42">
         <v>2.0576500000000001E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>26</v>
       </c>
@@ -4442,25 +3738,16 @@
         <v>5.4324400000000002E-4</v>
       </c>
       <c r="C43">
-        <v>26</v>
+        <v>4.1847500000000002E-4</v>
       </c>
       <c r="D43">
-        <v>4.1847500000000002E-4</v>
+        <v>1.4578400000000001E-4</v>
       </c>
       <c r="E43">
-        <v>26</v>
-      </c>
-      <c r="F43">
-        <v>1.4578400000000001E-4</v>
-      </c>
-      <c r="G43">
-        <v>26</v>
-      </c>
-      <c r="H43">
         <v>1.5225300000000001E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>27</v>
       </c>
@@ -4468,25 +3755,16 @@
         <v>4.1631300000000002E-4</v>
       </c>
       <c r="C44">
-        <v>27</v>
+        <v>3.2377099999999999E-4</v>
       </c>
       <c r="D44">
-        <v>3.2377099999999999E-4</v>
+        <v>1.06567E-4</v>
       </c>
       <c r="E44">
-        <v>27</v>
-      </c>
-      <c r="F44">
-        <v>1.06567E-4</v>
-      </c>
-      <c r="G44">
-        <v>27</v>
-      </c>
-      <c r="H44">
         <v>1.1267100000000001E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>28</v>
       </c>
@@ -4494,25 +3772,16 @@
         <v>3.2022000000000002E-4</v>
       </c>
       <c r="C45">
-        <v>28</v>
-      </c>
-      <c r="D45">
         <v>2.4727000000000001E-4</v>
       </c>
-      <c r="E45">
-        <v>28</v>
-      </c>
-      <c r="F45" s="2">
+      <c r="D45" s="2">
         <v>7.8003000000000005E-5</v>
       </c>
-      <c r="G45">
-        <v>28</v>
-      </c>
-      <c r="H45" s="2">
+      <c r="E45" s="2">
         <v>8.3395999999999999E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>29</v>
       </c>
@@ -4520,25 +3789,16 @@
         <v>2.4830300000000001E-4</v>
       </c>
       <c r="C46">
-        <v>29</v>
-      </c>
-      <c r="D46">
         <v>1.9431E-4</v>
       </c>
-      <c r="E46">
-        <v>29</v>
-      </c>
-      <c r="F46" s="2">
+      <c r="D46" s="2">
         <v>5.7166700000000003E-5</v>
       </c>
-      <c r="G46">
-        <v>29</v>
-      </c>
-      <c r="H46" s="2">
+      <c r="E46" s="2">
         <v>6.1743500000000003E-5</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>30</v>
       </c>
@@ -4546,25 +3806,16 @@
         <v>1.9066800000000001E-4</v>
       </c>
       <c r="C47">
-        <v>30</v>
-      </c>
-      <c r="D47">
         <v>1.4769499999999999E-4</v>
       </c>
-      <c r="E47">
-        <v>30</v>
-      </c>
-      <c r="F47" s="2">
+      <c r="D47" s="2">
         <v>4.19454E-5</v>
       </c>
-      <c r="G47">
-        <v>30</v>
-      </c>
-      <c r="H47" s="2">
+      <c r="E47" s="2">
         <v>4.5727099999999998E-5</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>31</v>
       </c>
@@ -4572,677 +3823,458 @@
         <v>1.48665E-4</v>
       </c>
       <c r="C48">
-        <v>31</v>
-      </c>
-      <c r="D48">
         <v>1.16574E-4</v>
       </c>
-      <c r="E48">
-        <v>31</v>
-      </c>
-      <c r="F48" s="2">
+      <c r="D48" s="2">
         <v>3.0905100000000003E-5</v>
       </c>
-      <c r="G48">
-        <v>31</v>
-      </c>
-      <c r="H48" s="2">
+      <c r="E48" s="2">
         <v>3.39877E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>32</v>
       </c>
       <c r="B49">
         <v>1.1501399999999999E-4</v>
       </c>
-      <c r="C49">
-        <v>32</v>
+      <c r="C49" s="2">
+        <v>8.8658200000000004E-5</v>
       </c>
       <c r="D49" s="2">
-        <v>8.8658200000000004E-5</v>
-      </c>
-      <c r="E49">
-        <v>32</v>
-      </c>
-      <c r="F49" s="2">
         <v>2.2881999999999999E-5</v>
       </c>
-      <c r="G49">
-        <v>32</v>
-      </c>
-      <c r="H49" s="2">
+      <c r="E49" s="2">
         <v>2.53193E-5</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>33</v>
       </c>
       <c r="B50" s="2">
         <v>8.9018999999999996E-5</v>
       </c>
-      <c r="C50">
-        <v>33</v>
+      <c r="C50" s="2">
+        <v>6.9952799999999999E-5</v>
       </c>
       <c r="D50" s="2">
-        <v>6.9952799999999999E-5</v>
-      </c>
-      <c r="E50">
-        <v>33</v>
-      </c>
-      <c r="F50" s="2">
         <v>1.6949899999999998E-5</v>
       </c>
-      <c r="G50">
-        <v>33</v>
-      </c>
-      <c r="H50" s="2">
+      <c r="E50" s="2">
         <v>1.89221E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>34</v>
       </c>
       <c r="B51" s="2">
         <v>6.9352300000000003E-5</v>
       </c>
-      <c r="C51">
-        <v>34</v>
+      <c r="C51" s="2">
+        <v>5.3499799999999999E-5</v>
       </c>
       <c r="D51" s="2">
-        <v>5.3499799999999999E-5</v>
-      </c>
-      <c r="E51">
-        <v>34</v>
-      </c>
-      <c r="F51" s="2">
         <v>1.25615E-5</v>
       </c>
-      <c r="G51">
-        <v>34</v>
-      </c>
-      <c r="H51" s="2">
+      <c r="E51" s="2">
         <v>1.4173699999999999E-5</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>35</v>
       </c>
       <c r="B52" s="2">
         <v>5.3328500000000003E-5</v>
       </c>
-      <c r="C52">
-        <v>35</v>
+      <c r="C52" s="2">
+        <v>4.2002200000000002E-5</v>
       </c>
       <c r="D52" s="2">
-        <v>4.2002200000000002E-5</v>
-      </c>
-      <c r="E52">
-        <v>35</v>
-      </c>
-      <c r="F52" s="2">
         <v>9.3136399999999995E-6</v>
       </c>
-      <c r="G52">
-        <v>35</v>
-      </c>
-      <c r="H52" s="2">
+      <c r="E52" s="2">
         <v>1.0615700000000001E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>36</v>
       </c>
       <c r="B53" s="2">
         <v>4.1819600000000002E-5</v>
       </c>
-      <c r="C53">
-        <v>36</v>
+      <c r="C53" s="2">
+        <v>3.2456899999999998E-5</v>
       </c>
       <c r="D53" s="2">
-        <v>3.2456899999999998E-5</v>
-      </c>
-      <c r="E53">
-        <v>36</v>
-      </c>
-      <c r="F53" s="2">
         <v>6.9086500000000003E-6</v>
       </c>
-      <c r="G53">
-        <v>36</v>
-      </c>
-      <c r="H53" s="2">
+      <c r="E53" s="2">
         <v>7.9504299999999997E-6</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>37</v>
       </c>
       <c r="B54" s="2">
         <v>3.19699E-5</v>
       </c>
-      <c r="C54">
-        <v>37</v>
+      <c r="C54" s="2">
+        <v>2.5241399999999999E-5</v>
       </c>
       <c r="D54" s="2">
-        <v>2.5241399999999999E-5</v>
-      </c>
-      <c r="E54">
-        <v>37</v>
-      </c>
-      <c r="F54" s="2">
         <v>5.1270799999999999E-6</v>
       </c>
-      <c r="G54">
-        <v>37</v>
-      </c>
-      <c r="H54" s="2">
+      <c r="E54" s="2">
         <v>5.9542700000000003E-6</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>38</v>
       </c>
       <c r="B55" s="2">
         <v>2.5224699999999999E-5</v>
       </c>
-      <c r="C55">
-        <v>38</v>
+      <c r="C55" s="2">
+        <v>1.9690600000000001E-5</v>
       </c>
       <c r="D55" s="2">
-        <v>1.9690600000000001E-5</v>
-      </c>
-      <c r="E55">
-        <v>38</v>
-      </c>
-      <c r="F55" s="2">
         <v>3.80618E-6</v>
       </c>
-      <c r="G55">
-        <v>38</v>
-      </c>
-      <c r="H55" s="2">
+      <c r="E55" s="2">
         <v>4.4594099999999999E-6</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>39</v>
       </c>
       <c r="B56" s="2">
         <v>1.9325800000000001E-5</v>
       </c>
-      <c r="C56">
-        <v>39</v>
+      <c r="C56" s="2">
+        <v>1.5330599999999999E-5</v>
       </c>
       <c r="D56" s="2">
-        <v>1.5330599999999999E-5</v>
-      </c>
-      <c r="E56">
-        <v>39</v>
-      </c>
-      <c r="F56" s="2">
         <v>2.8267099999999998E-6</v>
       </c>
-      <c r="G56">
-        <v>39</v>
-      </c>
-      <c r="H56" s="2">
+      <c r="E56" s="2">
         <v>3.3400499999999999E-6</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>40</v>
       </c>
       <c r="B57" s="2">
         <v>1.52225E-5</v>
       </c>
-      <c r="C57">
-        <v>40</v>
+      <c r="C57" s="2">
+        <v>1.19488E-5</v>
       </c>
       <c r="D57" s="2">
-        <v>1.19488E-5</v>
-      </c>
-      <c r="E57">
-        <v>40</v>
-      </c>
-      <c r="F57" s="2">
         <v>2.1003399999999999E-6</v>
       </c>
-      <c r="G57">
-        <v>40</v>
-      </c>
-      <c r="H57" s="2">
+      <c r="E57" s="2">
         <v>2.5018700000000002E-6</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>41</v>
       </c>
       <c r="B58" s="2">
         <v>1.17774E-5</v>
       </c>
-      <c r="C58">
-        <v>41</v>
+      <c r="C58" s="2">
+        <v>9.3875100000000002E-6</v>
       </c>
       <c r="D58" s="2">
-        <v>9.3875100000000002E-6</v>
-      </c>
-      <c r="E58">
-        <v>41</v>
-      </c>
-      <c r="F58" s="2">
         <v>1.56146E-6</v>
       </c>
-      <c r="G58">
-        <v>41</v>
-      </c>
-      <c r="H58" s="2">
+      <c r="E58" s="2">
         <v>1.87424E-6</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>42</v>
       </c>
       <c r="B59" s="2">
         <v>9.1921400000000007E-6</v>
       </c>
-      <c r="C59">
-        <v>42</v>
+      <c r="C59" s="2">
+        <v>7.2541200000000003E-6</v>
       </c>
       <c r="D59" s="2">
-        <v>7.2541200000000003E-6</v>
-      </c>
-      <c r="E59">
-        <v>42</v>
-      </c>
-      <c r="F59" s="2">
         <v>1.16103E-6</v>
       </c>
-      <c r="G59">
-        <v>42</v>
-      </c>
-      <c r="H59" s="2">
+      <c r="E59" s="2">
         <v>1.4042400000000001E-6</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>43</v>
       </c>
       <c r="B60" s="2">
         <v>7.1757700000000004E-6</v>
       </c>
-      <c r="C60">
-        <v>43</v>
+      <c r="C60" s="2">
+        <v>5.7466199999999999E-6</v>
       </c>
       <c r="D60" s="2">
-        <v>5.7466199999999999E-6</v>
-      </c>
-      <c r="E60">
-        <v>43</v>
-      </c>
-      <c r="F60" s="2">
         <v>8.6346599999999998E-7</v>
       </c>
-      <c r="G60">
-        <v>43</v>
-      </c>
-      <c r="H60" s="2">
+      <c r="E60" s="2">
         <v>1.05258E-6</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>44</v>
       </c>
       <c r="B61" s="2">
         <v>5.5547100000000002E-6</v>
       </c>
-      <c r="C61">
-        <v>44</v>
+      <c r="C61" s="2">
+        <v>4.4382400000000004E-6</v>
       </c>
       <c r="D61" s="2">
-        <v>4.4382400000000004E-6</v>
-      </c>
-      <c r="E61">
-        <v>44</v>
-      </c>
-      <c r="F61" s="2">
         <v>6.4247000000000001E-7</v>
       </c>
-      <c r="G61">
-        <v>44</v>
-      </c>
-      <c r="H61" s="2">
+      <c r="E61" s="2">
         <v>7.9141299999999999E-7</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>45</v>
       </c>
       <c r="B62" s="2">
         <v>4.3719800000000001E-6</v>
       </c>
-      <c r="C62">
-        <v>45</v>
+      <c r="C62" s="2">
+        <v>3.5175900000000001E-6</v>
       </c>
       <c r="D62" s="2">
-        <v>3.5175900000000001E-6</v>
-      </c>
-      <c r="E62">
-        <v>45</v>
-      </c>
-      <c r="F62" s="2">
         <v>4.7829399999999998E-7</v>
       </c>
-      <c r="G62">
-        <v>45</v>
-      </c>
-      <c r="H62" s="2">
+      <c r="E62" s="2">
         <v>5.9506799999999999E-7</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>46</v>
       </c>
       <c r="B63" s="2">
         <v>3.3592700000000002E-6</v>
       </c>
-      <c r="C63">
-        <v>46</v>
+      <c r="C63" s="2">
+        <v>2.71746E-6</v>
       </c>
       <c r="D63" s="2">
-        <v>2.71746E-6</v>
-      </c>
-      <c r="E63">
-        <v>46</v>
-      </c>
-      <c r="F63" s="2">
         <v>3.5606199999999998E-7</v>
       </c>
-      <c r="G63">
-        <v>46</v>
-      </c>
-      <c r="H63" s="2">
+      <c r="E63" s="2">
         <v>4.4847899999999998E-7</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>47</v>
       </c>
       <c r="B64" s="2">
         <v>2.6640600000000002E-6</v>
       </c>
-      <c r="C64">
-        <v>47</v>
+      <c r="C64" s="2">
+        <v>2.1533900000000001E-6</v>
       </c>
       <c r="D64" s="2">
-        <v>2.1533900000000001E-6</v>
-      </c>
-      <c r="E64">
-        <v>47</v>
-      </c>
-      <c r="F64" s="2">
         <v>2.6518100000000002E-7</v>
       </c>
-      <c r="G64">
-        <v>47</v>
-      </c>
-      <c r="H64" s="2">
+      <c r="E64" s="2">
         <v>3.3832999999999999E-7</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>48</v>
       </c>
       <c r="B65" s="2">
         <v>2.05042E-6</v>
       </c>
-      <c r="C65">
-        <v>48</v>
+      <c r="C65" s="2">
+        <v>1.6668700000000001E-6</v>
       </c>
       <c r="D65" s="2">
-        <v>1.6668700000000001E-6</v>
-      </c>
-      <c r="E65">
-        <v>48</v>
-      </c>
-      <c r="F65" s="2">
         <v>1.9777800000000001E-7</v>
       </c>
-      <c r="G65">
-        <v>48</v>
-      </c>
-      <c r="H65" s="2">
+      <c r="E65" s="2">
         <v>2.5522199999999998E-7</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>49</v>
       </c>
       <c r="B66" s="2">
         <v>1.62373E-6</v>
       </c>
-      <c r="C66">
-        <v>49</v>
+      <c r="C66" s="2">
+        <v>1.31857E-6</v>
       </c>
       <c r="D66" s="2">
-        <v>1.31857E-6</v>
-      </c>
-      <c r="E66">
-        <v>49</v>
-      </c>
-      <c r="F66" s="2">
         <v>1.4786700000000001E-7</v>
       </c>
-      <c r="G66">
-        <v>49</v>
-      </c>
-      <c r="H66" s="2">
+      <c r="E66" s="2">
         <v>1.9252400000000001E-7</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>50</v>
       </c>
       <c r="B67" s="2">
         <v>1.2556999999999999E-6</v>
       </c>
-      <c r="C67">
-        <v>50</v>
+      <c r="C67" s="2">
+        <v>1.0270399999999999E-6</v>
       </c>
       <c r="D67" s="2">
-        <v>1.0270399999999999E-6</v>
-      </c>
-      <c r="E67">
-        <v>50</v>
-      </c>
-      <c r="F67" s="2">
         <v>1.10543E-7</v>
       </c>
-      <c r="G67">
-        <v>50</v>
-      </c>
-      <c r="H67" s="2">
+      <c r="E67" s="2">
         <v>1.4522600000000001E-7</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>51</v>
       </c>
       <c r="B68" s="2">
         <v>9.8997299999999994E-7</v>
       </c>
-      <c r="C68">
-        <v>51</v>
+      <c r="C68" s="2">
+        <v>8.0766799999999998E-7</v>
       </c>
       <c r="D68" s="2">
-        <v>8.0766799999999998E-7</v>
-      </c>
-      <c r="E68">
-        <v>51</v>
-      </c>
-      <c r="F68" s="2">
         <v>8.2689799999999997E-8</v>
       </c>
-      <c r="G68">
-        <v>51</v>
-      </c>
-      <c r="H68" s="2">
+      <c r="E68" s="2">
         <v>1.09549E-7</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>52</v>
       </c>
       <c r="B69" s="2">
         <v>7.6906499999999996E-7</v>
       </c>
-      <c r="C69">
-        <v>52</v>
-      </c>
-      <c r="D69" s="2">
+      <c r="C69" s="2">
         <v>6.3277999999999998E-7</v>
       </c>
-      <c r="G69">
-        <v>52</v>
-      </c>
-      <c r="H69" s="2">
+      <c r="E69" s="2">
         <v>8.2638000000000002E-8</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>53</v>
       </c>
       <c r="B70" s="2">
         <v>6.0381199999999995E-7</v>
       </c>
-      <c r="C70">
-        <v>53</v>
-      </c>
-      <c r="D70" s="2">
+      <c r="C70" s="2">
         <v>4.9492800000000005E-7</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>54</v>
       </c>
       <c r="B71" s="2">
         <v>4.7109600000000003E-7</v>
       </c>
-      <c r="C71">
-        <v>54</v>
-      </c>
-      <c r="D71" s="2">
+      <c r="C71" s="2">
         <v>3.8988899999999998E-7</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>55</v>
       </c>
       <c r="B72" s="2">
         <v>3.6844199999999998E-7</v>
       </c>
-      <c r="C72">
-        <v>55</v>
-      </c>
-      <c r="D72" s="2">
+      <c r="C72" s="2">
         <v>3.0643799999999998E-7</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>56</v>
       </c>
       <c r="B73" s="2">
         <v>2.8863800000000002E-7</v>
       </c>
-      <c r="C73">
-        <v>56</v>
-      </c>
-      <c r="D73" s="2">
+      <c r="C73" s="2">
         <v>2.4026600000000002E-7</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>57</v>
       </c>
       <c r="B74" s="2">
         <v>2.2492999999999999E-7</v>
       </c>
-      <c r="C74">
-        <v>57</v>
-      </c>
-      <c r="D74" s="2">
+      <c r="C74" s="2">
         <v>1.8986000000000001E-7</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>58</v>
       </c>
       <c r="B75" s="2">
         <v>1.76895E-7</v>
       </c>
-      <c r="C75">
-        <v>58</v>
-      </c>
-      <c r="D75" s="2">
+      <c r="C75" s="2">
         <v>1.48094E-7</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>59</v>
       </c>
       <c r="B76" s="2">
         <v>1.38589E-7</v>
       </c>
-      <c r="C76">
-        <v>59</v>
-      </c>
-      <c r="D76" s="2">
+      <c r="C76" s="2">
         <v>1.17619E-7</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:5">
       <c r="A77">
         <v>60</v>
       </c>
       <c r="B77" s="2">
         <v>1.08445E-7</v>
       </c>
-      <c r="C77">
-        <v>60</v>
-      </c>
-      <c r="D77" s="2">
+      <c r="C77" s="2">
         <v>9.1701799999999999E-8</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Updates to the jcomp2012 paper
</commit_message>
<xml_diff>
--- a/doc/hmcsa_adjoint_vs_direct/direct_vs_adjoint.xlsx
+++ b/doc/hmcsa_adjoint_vs_direct/direct_vs_adjoint.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>problem parameters</t>
   </si>
@@ -154,8 +154,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -196,7 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -213,6 +231,15 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -229,6 +256,15 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1267,7 +1303,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Convergence Study'!$B$16</c:f>
+              <c:f>'Convergence Study'!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1677,11 +1713,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Convergence Study'!#REF!</c:f>
+              <c:f>'Convergence Study'!$C$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>#REF!</c:v>
+                  <c:v>Direct 5 Point</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1698,12 +1734,196 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Convergence Study'!#REF!</c:f>
+              <c:f>'Convergence Study'!$C$18:$C$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60.0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Convergence Study'!$C$18:$C$77</c:f>
+              <c:f>'Convergence Study'!$D$18:$D$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -1897,7 +2117,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Convergence Study'!$D$16</c:f>
+              <c:f>'Convergence Study'!$E$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1918,12 +2138,169 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Convergence Study'!#REF!</c:f>
+              <c:f>'Convergence Study'!$E$18:$E$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51.0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Convergence Study'!$D$18:$D$68</c:f>
+              <c:f>'Convergence Study'!$F$18:$F$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2090,7 +2467,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Convergence Study'!$E$16</c:f>
+              <c:f>'Convergence Study'!$G$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2113,12 +2490,172 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Convergence Study'!#REF!</c:f>
+              <c:f>'Convergence Study'!$G$18:$G$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52.0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Convergence Study'!$E$18:$E$69</c:f>
+              <c:f>'Convergence Study'!$H$18:$H$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
@@ -2460,13 +2997,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>177800</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>711200</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -3156,45 +3693,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G18" sqref="G18:H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3202,7 +3739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3210,7 +3747,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3218,7 +3755,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3226,7 +3763,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3234,7 +3771,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3242,7 +3779,7 @@
         <v>1E-8</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3250,7 +3787,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3258,7 +3795,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -3266,7 +3803,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3274,21 +3811,21 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="1:7">
+      <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3296,16 +3833,25 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
       </c>
       <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3313,16 +3859,25 @@
         <v>4</v>
       </c>
       <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
         <v>4</v>
       </c>
-      <c r="D18">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
         <v>4.2307699999999997</v>
       </c>
-      <c r="E18">
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
         <v>4.2307699999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3330,16 +3885,25 @@
         <v>3.0655000000000001</v>
       </c>
       <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
         <v>1.2</v>
       </c>
-      <c r="D19">
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
         <v>4.1364099999999997</v>
       </c>
-      <c r="E19">
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
         <v>1.09467</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>3</v>
       </c>
@@ -3347,16 +3911,25 @@
         <v>1.5100800000000001</v>
       </c>
       <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
         <v>0.64</v>
       </c>
-      <c r="D20">
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
         <v>1.62737</v>
       </c>
-      <c r="E20">
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
         <v>0.58261300000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>4</v>
       </c>
@@ -3364,16 +3937,25 @@
         <v>0.827511</v>
       </c>
       <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
         <v>0.35199999999999998</v>
       </c>
-      <c r="D21">
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
         <v>0.62627100000000002</v>
       </c>
-      <c r="E21">
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
         <v>0.32868199999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>5</v>
       </c>
@@ -3381,16 +3963,25 @@
         <v>0.45778999999999997</v>
       </c>
       <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
         <v>0.25600000000000001</v>
       </c>
-      <c r="D22">
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
         <v>0.37118200000000001</v>
       </c>
-      <c r="E22">
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
         <v>0.19822600000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>6</v>
       </c>
@@ -3398,16 +3989,25 @@
         <v>0.32209500000000002</v>
       </c>
       <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
         <v>0.15679999999999999</v>
       </c>
-      <c r="D23">
+      <c r="E23">
+        <v>6</v>
+      </c>
+      <c r="F23">
         <v>0.22998499999999999</v>
       </c>
-      <c r="E23">
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
         <v>0.122722</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>7</v>
       </c>
@@ -3415,16 +4015,25 @@
         <v>0.191576</v>
       </c>
       <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
         <v>0.10752</v>
       </c>
-      <c r="D24">
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
         <v>0.13960800000000001</v>
       </c>
-      <c r="E24">
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="H24">
         <v>8.1978099999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>8</v>
       </c>
@@ -3432,16 +4041,25 @@
         <v>0.13731199999999999</v>
       </c>
       <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
         <v>7.5263999999999998E-2</v>
       </c>
-      <c r="D25">
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25">
         <v>8.9023000000000005E-2</v>
       </c>
-      <c r="E25">
+      <c r="G25">
+        <v>8</v>
+      </c>
+      <c r="H25">
         <v>5.6275899999999997E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>9</v>
       </c>
@@ -3449,16 +4067,25 @@
         <v>9.1996599999999998E-2</v>
       </c>
       <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
         <v>5.5050200000000001E-2</v>
       </c>
-      <c r="D26">
+      <c r="E26">
+        <v>9</v>
+      </c>
+      <c r="F26">
         <v>5.6296800000000001E-2</v>
       </c>
-      <c r="E26">
+      <c r="G26">
+        <v>9</v>
+      </c>
+      <c r="H26">
         <v>3.8681599999999997E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>10</v>
       </c>
@@ -3466,16 +4093,25 @@
         <v>6.32601E-2</v>
       </c>
       <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
         <v>3.7933099999999997E-2</v>
       </c>
-      <c r="D27">
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
         <v>3.66427E-2</v>
       </c>
-      <c r="E27">
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="H27">
         <v>2.6579700000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>11</v>
       </c>
@@ -3483,16 +4119,25 @@
         <v>4.5238500000000001E-2</v>
       </c>
       <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
         <v>2.9196300000000001E-2</v>
       </c>
-      <c r="D28">
+      <c r="E28">
+        <v>11</v>
+      </c>
+      <c r="F28">
         <v>2.4831300000000001E-2</v>
       </c>
-      <c r="E28">
+      <c r="G28">
+        <v>11</v>
+      </c>
+      <c r="H28">
         <v>1.83421E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>12</v>
       </c>
@@ -3500,16 +4145,25 @@
         <v>3.2290300000000001E-2</v>
       </c>
       <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
         <v>2.0295500000000001E-2</v>
       </c>
-      <c r="D29">
+      <c r="E29">
+        <v>12</v>
+      </c>
+      <c r="F29">
         <v>1.69751E-2</v>
       </c>
-      <c r="E29">
+      <c r="G29">
+        <v>12</v>
+      </c>
+      <c r="H29">
         <v>1.2773400000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>13</v>
       </c>
@@ -3517,16 +4171,25 @@
         <v>2.3428899999999999E-2</v>
       </c>
       <c r="C30">
+        <v>13</v>
+      </c>
+      <c r="D30">
         <v>1.55405E-2</v>
       </c>
-      <c r="D30">
+      <c r="E30">
+        <v>13</v>
+      </c>
+      <c r="F30">
         <v>1.1687299999999999E-2</v>
       </c>
-      <c r="E30">
+      <c r="G30">
+        <v>13</v>
+      </c>
+      <c r="H30">
         <v>9.0492100000000002E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>14</v>
       </c>
@@ -3534,16 +4197,25 @@
         <v>1.73023E-2</v>
       </c>
       <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31">
         <v>1.13242E-2</v>
       </c>
-      <c r="D31">
+      <c r="E31">
+        <v>14</v>
+      </c>
+      <c r="F31">
         <v>8.0797100000000004E-3</v>
       </c>
-      <c r="E31">
+      <c r="G31">
+        <v>14</v>
+      </c>
+      <c r="H31">
         <v>6.5498199999999996E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>15</v>
       </c>
@@ -3551,16 +4223,25 @@
         <v>1.25367E-2</v>
       </c>
       <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32">
         <v>8.3491099999999999E-3</v>
       </c>
-      <c r="D32">
+      <c r="E32">
+        <v>15</v>
+      </c>
+      <c r="F32">
         <v>5.6182999999999997E-3</v>
       </c>
-      <c r="E32">
+      <c r="G32">
+        <v>15</v>
+      </c>
+      <c r="H32">
         <v>4.7388999999999999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>16</v>
       </c>
@@ -3568,16 +4249,25 @@
         <v>9.3289900000000005E-3</v>
       </c>
       <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33">
         <v>6.3210999999999996E-3</v>
       </c>
-      <c r="D33">
+      <c r="E33">
+        <v>16</v>
+      </c>
+      <c r="F33">
         <v>3.9245299999999999E-3</v>
       </c>
-      <c r="E33">
+      <c r="G33">
+        <v>16</v>
+      </c>
+      <c r="H33">
         <v>3.4273200000000002E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>17</v>
       </c>
@@ -3585,16 +4275,25 @@
         <v>6.7580699999999997E-3</v>
       </c>
       <c r="C34">
+        <v>17</v>
+      </c>
+      <c r="D34">
         <v>4.82491E-3</v>
       </c>
-      <c r="D34">
+      <c r="E34">
+        <v>17</v>
+      </c>
+      <c r="F34">
         <v>2.7549499999999999E-3</v>
       </c>
-      <c r="E34">
+      <c r="G34">
+        <v>17</v>
+      </c>
+      <c r="H34">
         <v>2.4792400000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>18</v>
       </c>
@@ -3602,16 +4301,25 @@
         <v>5.0667999999999998E-3</v>
       </c>
       <c r="C35">
+        <v>18</v>
+      </c>
+      <c r="D35">
         <v>3.5581599999999999E-3</v>
       </c>
-      <c r="D35">
+      <c r="E35">
+        <v>18</v>
+      </c>
+      <c r="F35">
         <v>1.9422300000000001E-3</v>
       </c>
-      <c r="E35">
+      <c r="G35">
+        <v>18</v>
+      </c>
+      <c r="H35">
         <v>1.79433E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>19</v>
       </c>
@@ -3619,16 +4327,25 @@
         <v>3.6701199999999998E-3</v>
       </c>
       <c r="C36">
+        <v>19</v>
+      </c>
+      <c r="D36">
         <v>2.7880299999999999E-3</v>
       </c>
-      <c r="D36">
+      <c r="E36">
+        <v>19</v>
+      </c>
+      <c r="F36">
         <v>1.3750399999999999E-3</v>
       </c>
-      <c r="E36">
+      <c r="G36">
+        <v>19</v>
+      </c>
+      <c r="H36">
         <v>1.29963E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>20</v>
       </c>
@@ -3636,16 +4353,25 @@
         <v>2.7727400000000001E-3</v>
       </c>
       <c r="C37">
+        <v>20</v>
+      </c>
+      <c r="D37">
         <v>2.0581499999999999E-3</v>
       </c>
-      <c r="D37">
+      <c r="E37">
+        <v>20</v>
+      </c>
+      <c r="F37">
         <v>9.8730100000000011E-4</v>
       </c>
-      <c r="E37">
+      <c r="G37">
+        <v>20</v>
+      </c>
+      <c r="H37">
         <v>9.4218600000000002E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>21</v>
       </c>
@@ -3653,16 +4379,25 @@
         <v>2.0073299999999999E-3</v>
       </c>
       <c r="C38">
+        <v>21</v>
+      </c>
+      <c r="D38">
         <v>1.6110199999999999E-3</v>
       </c>
-      <c r="D38">
+      <c r="E38">
+        <v>21</v>
+      </c>
+      <c r="F38">
         <v>7.1468200000000001E-4</v>
       </c>
-      <c r="E38">
+      <c r="G38">
+        <v>21</v>
+      </c>
+      <c r="H38">
         <v>6.90367E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>22</v>
       </c>
@@ -3670,16 +4405,25 @@
         <v>1.5676799999999999E-3</v>
       </c>
       <c r="C39">
+        <v>22</v>
+      </c>
+      <c r="D39">
         <v>1.2010600000000001E-3</v>
       </c>
-      <c r="D39">
+      <c r="E39">
+        <v>22</v>
+      </c>
+      <c r="F39">
         <v>5.1829999999999997E-4</v>
       </c>
-      <c r="E39">
+      <c r="G39">
+        <v>22</v>
+      </c>
+      <c r="H39">
         <v>5.07643E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>23</v>
       </c>
@@ -3687,16 +4431,25 @@
         <v>1.1850700000000001E-3</v>
       </c>
       <c r="C40">
+        <v>23</v>
+      </c>
+      <c r="D40">
         <v>9.32441E-4</v>
       </c>
-      <c r="D40">
+      <c r="E40">
+        <v>23</v>
+      </c>
+      <c r="F40">
         <v>3.7653799999999999E-4</v>
       </c>
-      <c r="E40">
+      <c r="G40">
+        <v>23</v>
+      </c>
+      <c r="H40">
         <v>3.7577900000000002E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>24</v>
       </c>
@@ -3704,16 +4457,25 @@
         <v>9.2259700000000004E-4</v>
       </c>
       <c r="C41">
+        <v>24</v>
+      </c>
+      <c r="D41">
         <v>7.0889599999999998E-4</v>
       </c>
-      <c r="D41">
+      <c r="E41">
+        <v>24</v>
+      </c>
+      <c r="F41">
         <v>2.7400999999999999E-4</v>
       </c>
-      <c r="E41">
+      <c r="G41">
+        <v>24</v>
+      </c>
+      <c r="H41">
         <v>2.7808599999999998E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>25</v>
       </c>
@@ -3721,16 +4483,25 @@
         <v>7.0223400000000004E-4</v>
       </c>
       <c r="C42">
+        <v>25</v>
+      </c>
+      <c r="D42">
         <v>5.4104200000000004E-4</v>
       </c>
-      <c r="D42">
+      <c r="E42">
+        <v>25</v>
+      </c>
+      <c r="F42">
         <v>1.9971600000000001E-4</v>
       </c>
-      <c r="E42">
+      <c r="G42">
+        <v>25</v>
+      </c>
+      <c r="H42">
         <v>2.0576500000000001E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>26</v>
       </c>
@@ -3738,16 +4509,25 @@
         <v>5.4324400000000002E-4</v>
       </c>
       <c r="C43">
+        <v>26</v>
+      </c>
+      <c r="D43">
         <v>4.1847500000000002E-4</v>
       </c>
-      <c r="D43">
+      <c r="E43">
+        <v>26</v>
+      </c>
+      <c r="F43">
         <v>1.4578400000000001E-4</v>
       </c>
-      <c r="E43">
+      <c r="G43">
+        <v>26</v>
+      </c>
+      <c r="H43">
         <v>1.5225300000000001E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>27</v>
       </c>
@@ -3755,16 +4535,25 @@
         <v>4.1631300000000002E-4</v>
       </c>
       <c r="C44">
+        <v>27</v>
+      </c>
+      <c r="D44">
         <v>3.2377099999999999E-4</v>
       </c>
-      <c r="D44">
+      <c r="E44">
+        <v>27</v>
+      </c>
+      <c r="F44">
         <v>1.06567E-4</v>
       </c>
-      <c r="E44">
+      <c r="G44">
+        <v>27</v>
+      </c>
+      <c r="H44">
         <v>1.1267100000000001E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>28</v>
       </c>
@@ -3772,16 +4561,25 @@
         <v>3.2022000000000002E-4</v>
       </c>
       <c r="C45">
+        <v>28</v>
+      </c>
+      <c r="D45">
         <v>2.4727000000000001E-4</v>
       </c>
-      <c r="D45" s="2">
+      <c r="E45">
+        <v>28</v>
+      </c>
+      <c r="F45" s="2">
         <v>7.8003000000000005E-5</v>
       </c>
-      <c r="E45" s="2">
+      <c r="G45">
+        <v>28</v>
+      </c>
+      <c r="H45" s="2">
         <v>8.3395999999999999E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>29</v>
       </c>
@@ -3789,16 +4587,25 @@
         <v>2.4830300000000001E-4</v>
       </c>
       <c r="C46">
+        <v>29</v>
+      </c>
+      <c r="D46">
         <v>1.9431E-4</v>
       </c>
-      <c r="D46" s="2">
+      <c r="E46">
+        <v>29</v>
+      </c>
+      <c r="F46" s="2">
         <v>5.7166700000000003E-5</v>
       </c>
-      <c r="E46" s="2">
+      <c r="G46">
+        <v>29</v>
+      </c>
+      <c r="H46" s="2">
         <v>6.1743500000000003E-5</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>30</v>
       </c>
@@ -3806,16 +4613,25 @@
         <v>1.9066800000000001E-4</v>
       </c>
       <c r="C47">
+        <v>30</v>
+      </c>
+      <c r="D47">
         <v>1.4769499999999999E-4</v>
       </c>
-      <c r="D47" s="2">
+      <c r="E47">
+        <v>30</v>
+      </c>
+      <c r="F47" s="2">
         <v>4.19454E-5</v>
       </c>
-      <c r="E47" s="2">
+      <c r="G47">
+        <v>30</v>
+      </c>
+      <c r="H47" s="2">
         <v>4.5727099999999998E-5</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>31</v>
       </c>
@@ -3823,458 +4639,677 @@
         <v>1.48665E-4</v>
       </c>
       <c r="C48">
+        <v>31</v>
+      </c>
+      <c r="D48">
         <v>1.16574E-4</v>
       </c>
-      <c r="D48" s="2">
+      <c r="E48">
+        <v>31</v>
+      </c>
+      <c r="F48" s="2">
         <v>3.0905100000000003E-5</v>
       </c>
-      <c r="E48" s="2">
+      <c r="G48">
+        <v>31</v>
+      </c>
+      <c r="H48" s="2">
         <v>3.39877E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:8">
       <c r="A49">
         <v>32</v>
       </c>
       <c r="B49">
         <v>1.1501399999999999E-4</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49">
+        <v>32</v>
+      </c>
+      <c r="D49" s="2">
         <v>8.8658200000000004E-5</v>
       </c>
-      <c r="D49" s="2">
+      <c r="E49">
+        <v>32</v>
+      </c>
+      <c r="F49" s="2">
         <v>2.2881999999999999E-5</v>
       </c>
-      <c r="E49" s="2">
+      <c r="G49">
+        <v>32</v>
+      </c>
+      <c r="H49" s="2">
         <v>2.53193E-5</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:8">
       <c r="A50">
         <v>33</v>
       </c>
       <c r="B50" s="2">
         <v>8.9018999999999996E-5</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50">
+        <v>33</v>
+      </c>
+      <c r="D50" s="2">
         <v>6.9952799999999999E-5</v>
       </c>
-      <c r="D50" s="2">
+      <c r="E50">
+        <v>33</v>
+      </c>
+      <c r="F50" s="2">
         <v>1.6949899999999998E-5</v>
       </c>
-      <c r="E50" s="2">
+      <c r="G50">
+        <v>33</v>
+      </c>
+      <c r="H50" s="2">
         <v>1.89221E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>34</v>
       </c>
       <c r="B51" s="2">
         <v>6.9352300000000003E-5</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51">
+        <v>34</v>
+      </c>
+      <c r="D51" s="2">
         <v>5.3499799999999999E-5</v>
       </c>
-      <c r="D51" s="2">
+      <c r="E51">
+        <v>34</v>
+      </c>
+      <c r="F51" s="2">
         <v>1.25615E-5</v>
       </c>
-      <c r="E51" s="2">
+      <c r="G51">
+        <v>34</v>
+      </c>
+      <c r="H51" s="2">
         <v>1.4173699999999999E-5</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:8">
       <c r="A52">
         <v>35</v>
       </c>
       <c r="B52" s="2">
         <v>5.3328500000000003E-5</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52">
+        <v>35</v>
+      </c>
+      <c r="D52" s="2">
         <v>4.2002200000000002E-5</v>
       </c>
-      <c r="D52" s="2">
+      <c r="E52">
+        <v>35</v>
+      </c>
+      <c r="F52" s="2">
         <v>9.3136399999999995E-6</v>
       </c>
-      <c r="E52" s="2">
+      <c r="G52">
+        <v>35</v>
+      </c>
+      <c r="H52" s="2">
         <v>1.0615700000000001E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:8">
       <c r="A53">
         <v>36</v>
       </c>
       <c r="B53" s="2">
         <v>4.1819600000000002E-5</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53">
+        <v>36</v>
+      </c>
+      <c r="D53" s="2">
         <v>3.2456899999999998E-5</v>
       </c>
-      <c r="D53" s="2">
+      <c r="E53">
+        <v>36</v>
+      </c>
+      <c r="F53" s="2">
         <v>6.9086500000000003E-6</v>
       </c>
-      <c r="E53" s="2">
+      <c r="G53">
+        <v>36</v>
+      </c>
+      <c r="H53" s="2">
         <v>7.9504299999999997E-6</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:8">
       <c r="A54">
         <v>37</v>
       </c>
       <c r="B54" s="2">
         <v>3.19699E-5</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54">
+        <v>37</v>
+      </c>
+      <c r="D54" s="2">
         <v>2.5241399999999999E-5</v>
       </c>
-      <c r="D54" s="2">
+      <c r="E54">
+        <v>37</v>
+      </c>
+      <c r="F54" s="2">
         <v>5.1270799999999999E-6</v>
       </c>
-      <c r="E54" s="2">
+      <c r="G54">
+        <v>37</v>
+      </c>
+      <c r="H54" s="2">
         <v>5.9542700000000003E-6</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:8">
       <c r="A55">
         <v>38</v>
       </c>
       <c r="B55" s="2">
         <v>2.5224699999999999E-5</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55">
+        <v>38</v>
+      </c>
+      <c r="D55" s="2">
         <v>1.9690600000000001E-5</v>
       </c>
-      <c r="D55" s="2">
+      <c r="E55">
+        <v>38</v>
+      </c>
+      <c r="F55" s="2">
         <v>3.80618E-6</v>
       </c>
-      <c r="E55" s="2">
+      <c r="G55">
+        <v>38</v>
+      </c>
+      <c r="H55" s="2">
         <v>4.4594099999999999E-6</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:8">
       <c r="A56">
         <v>39</v>
       </c>
       <c r="B56" s="2">
         <v>1.9325800000000001E-5</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56">
+        <v>39</v>
+      </c>
+      <c r="D56" s="2">
         <v>1.5330599999999999E-5</v>
       </c>
-      <c r="D56" s="2">
+      <c r="E56">
+        <v>39</v>
+      </c>
+      <c r="F56" s="2">
         <v>2.8267099999999998E-6</v>
       </c>
-      <c r="E56" s="2">
+      <c r="G56">
+        <v>39</v>
+      </c>
+      <c r="H56" s="2">
         <v>3.3400499999999999E-6</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:8">
       <c r="A57">
         <v>40</v>
       </c>
       <c r="B57" s="2">
         <v>1.52225E-5</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57">
+        <v>40</v>
+      </c>
+      <c r="D57" s="2">
         <v>1.19488E-5</v>
       </c>
-      <c r="D57" s="2">
+      <c r="E57">
+        <v>40</v>
+      </c>
+      <c r="F57" s="2">
         <v>2.1003399999999999E-6</v>
       </c>
-      <c r="E57" s="2">
+      <c r="G57">
+        <v>40</v>
+      </c>
+      <c r="H57" s="2">
         <v>2.5018700000000002E-6</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:8">
       <c r="A58">
         <v>41</v>
       </c>
       <c r="B58" s="2">
         <v>1.17774E-5</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58">
+        <v>41</v>
+      </c>
+      <c r="D58" s="2">
         <v>9.3875100000000002E-6</v>
       </c>
-      <c r="D58" s="2">
+      <c r="E58">
+        <v>41</v>
+      </c>
+      <c r="F58" s="2">
         <v>1.56146E-6</v>
       </c>
-      <c r="E58" s="2">
+      <c r="G58">
+        <v>41</v>
+      </c>
+      <c r="H58" s="2">
         <v>1.87424E-6</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:8">
       <c r="A59">
         <v>42</v>
       </c>
       <c r="B59" s="2">
         <v>9.1921400000000007E-6</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59">
+        <v>42</v>
+      </c>
+      <c r="D59" s="2">
         <v>7.2541200000000003E-6</v>
       </c>
-      <c r="D59" s="2">
+      <c r="E59">
+        <v>42</v>
+      </c>
+      <c r="F59" s="2">
         <v>1.16103E-6</v>
       </c>
-      <c r="E59" s="2">
+      <c r="G59">
+        <v>42</v>
+      </c>
+      <c r="H59" s="2">
         <v>1.4042400000000001E-6</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:8">
       <c r="A60">
         <v>43</v>
       </c>
       <c r="B60" s="2">
         <v>7.1757700000000004E-6</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60">
+        <v>43</v>
+      </c>
+      <c r="D60" s="2">
         <v>5.7466199999999999E-6</v>
       </c>
-      <c r="D60" s="2">
+      <c r="E60">
+        <v>43</v>
+      </c>
+      <c r="F60" s="2">
         <v>8.6346599999999998E-7</v>
       </c>
-      <c r="E60" s="2">
+      <c r="G60">
+        <v>43</v>
+      </c>
+      <c r="H60" s="2">
         <v>1.05258E-6</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:8">
       <c r="A61">
         <v>44</v>
       </c>
       <c r="B61" s="2">
         <v>5.5547100000000002E-6</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61">
+        <v>44</v>
+      </c>
+      <c r="D61" s="2">
         <v>4.4382400000000004E-6</v>
       </c>
-      <c r="D61" s="2">
+      <c r="E61">
+        <v>44</v>
+      </c>
+      <c r="F61" s="2">
         <v>6.4247000000000001E-7</v>
       </c>
-      <c r="E61" s="2">
+      <c r="G61">
+        <v>44</v>
+      </c>
+      <c r="H61" s="2">
         <v>7.9141299999999999E-7</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:8">
       <c r="A62">
         <v>45</v>
       </c>
       <c r="B62" s="2">
         <v>4.3719800000000001E-6</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62">
+        <v>45</v>
+      </c>
+      <c r="D62" s="2">
         <v>3.5175900000000001E-6</v>
       </c>
-      <c r="D62" s="2">
+      <c r="E62">
+        <v>45</v>
+      </c>
+      <c r="F62" s="2">
         <v>4.7829399999999998E-7</v>
       </c>
-      <c r="E62" s="2">
+      <c r="G62">
+        <v>45</v>
+      </c>
+      <c r="H62" s="2">
         <v>5.9506799999999999E-7</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:8">
       <c r="A63">
         <v>46</v>
       </c>
       <c r="B63" s="2">
         <v>3.3592700000000002E-6</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63">
+        <v>46</v>
+      </c>
+      <c r="D63" s="2">
         <v>2.71746E-6</v>
       </c>
-      <c r="D63" s="2">
+      <c r="E63">
+        <v>46</v>
+      </c>
+      <c r="F63" s="2">
         <v>3.5606199999999998E-7</v>
       </c>
-      <c r="E63" s="2">
+      <c r="G63">
+        <v>46</v>
+      </c>
+      <c r="H63" s="2">
         <v>4.4847899999999998E-7</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:8">
       <c r="A64">
         <v>47</v>
       </c>
       <c r="B64" s="2">
         <v>2.6640600000000002E-6</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64">
+        <v>47</v>
+      </c>
+      <c r="D64" s="2">
         <v>2.1533900000000001E-6</v>
       </c>
-      <c r="D64" s="2">
+      <c r="E64">
+        <v>47</v>
+      </c>
+      <c r="F64" s="2">
         <v>2.6518100000000002E-7</v>
       </c>
-      <c r="E64" s="2">
+      <c r="G64">
+        <v>47</v>
+      </c>
+      <c r="H64" s="2">
         <v>3.3832999999999999E-7</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:8">
       <c r="A65">
         <v>48</v>
       </c>
       <c r="B65" s="2">
         <v>2.05042E-6</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65">
+        <v>48</v>
+      </c>
+      <c r="D65" s="2">
         <v>1.6668700000000001E-6</v>
       </c>
-      <c r="D65" s="2">
+      <c r="E65">
+        <v>48</v>
+      </c>
+      <c r="F65" s="2">
         <v>1.9777800000000001E-7</v>
       </c>
-      <c r="E65" s="2">
+      <c r="G65">
+        <v>48</v>
+      </c>
+      <c r="H65" s="2">
         <v>2.5522199999999998E-7</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:8">
       <c r="A66">
         <v>49</v>
       </c>
       <c r="B66" s="2">
         <v>1.62373E-6</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66">
+        <v>49</v>
+      </c>
+      <c r="D66" s="2">
         <v>1.31857E-6</v>
       </c>
-      <c r="D66" s="2">
+      <c r="E66">
+        <v>49</v>
+      </c>
+      <c r="F66" s="2">
         <v>1.4786700000000001E-7</v>
       </c>
-      <c r="E66" s="2">
+      <c r="G66">
+        <v>49</v>
+      </c>
+      <c r="H66" s="2">
         <v>1.9252400000000001E-7</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:8">
       <c r="A67">
         <v>50</v>
       </c>
       <c r="B67" s="2">
         <v>1.2556999999999999E-6</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67">
+        <v>50</v>
+      </c>
+      <c r="D67" s="2">
         <v>1.0270399999999999E-6</v>
       </c>
-      <c r="D67" s="2">
+      <c r="E67">
+        <v>50</v>
+      </c>
+      <c r="F67" s="2">
         <v>1.10543E-7</v>
       </c>
-      <c r="E67" s="2">
+      <c r="G67">
+        <v>50</v>
+      </c>
+      <c r="H67" s="2">
         <v>1.4522600000000001E-7</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:8">
       <c r="A68">
         <v>51</v>
       </c>
       <c r="B68" s="2">
         <v>9.8997299999999994E-7</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68">
+        <v>51</v>
+      </c>
+      <c r="D68" s="2">
         <v>8.0766799999999998E-7</v>
       </c>
-      <c r="D68" s="2">
+      <c r="E68">
+        <v>51</v>
+      </c>
+      <c r="F68" s="2">
         <v>8.2689799999999997E-8</v>
       </c>
-      <c r="E68" s="2">
+      <c r="G68">
+        <v>51</v>
+      </c>
+      <c r="H68" s="2">
         <v>1.09549E-7</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:8">
       <c r="A69">
         <v>52</v>
       </c>
       <c r="B69" s="2">
         <v>7.6906499999999996E-7</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69">
+        <v>52</v>
+      </c>
+      <c r="D69" s="2">
         <v>6.3277999999999998E-7</v>
       </c>
-      <c r="E69" s="2">
+      <c r="G69">
+        <v>52</v>
+      </c>
+      <c r="H69" s="2">
         <v>8.2638000000000002E-8</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:8">
       <c r="A70">
         <v>53</v>
       </c>
       <c r="B70" s="2">
         <v>6.0381199999999995E-7</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70">
+        <v>53</v>
+      </c>
+      <c r="D70" s="2">
         <v>4.9492800000000005E-7</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:8">
       <c r="A71">
         <v>54</v>
       </c>
       <c r="B71" s="2">
         <v>4.7109600000000003E-7</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71">
+        <v>54</v>
+      </c>
+      <c r="D71" s="2">
         <v>3.8988899999999998E-7</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:8">
       <c r="A72">
         <v>55</v>
       </c>
       <c r="B72" s="2">
         <v>3.6844199999999998E-7</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72">
+        <v>55</v>
+      </c>
+      <c r="D72" s="2">
         <v>3.0643799999999998E-7</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:8">
       <c r="A73">
         <v>56</v>
       </c>
       <c r="B73" s="2">
         <v>2.8863800000000002E-7</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73">
+        <v>56</v>
+      </c>
+      <c r="D73" s="2">
         <v>2.4026600000000002E-7</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:8">
       <c r="A74">
         <v>57</v>
       </c>
       <c r="B74" s="2">
         <v>2.2492999999999999E-7</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74">
+        <v>57</v>
+      </c>
+      <c r="D74" s="2">
         <v>1.8986000000000001E-7</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:8">
       <c r="A75">
         <v>58</v>
       </c>
       <c r="B75" s="2">
         <v>1.76895E-7</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75">
+        <v>58</v>
+      </c>
+      <c r="D75" s="2">
         <v>1.48094E-7</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:8">
       <c r="A76">
         <v>59</v>
       </c>
       <c r="B76" s="2">
         <v>1.38589E-7</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76">
+        <v>59</v>
+      </c>
+      <c r="D76" s="2">
         <v>1.17619E-7</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:8">
       <c r="A77">
         <v>60</v>
       </c>
       <c r="B77" s="2">
         <v>1.08445E-7</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77">
+        <v>60</v>
+      </c>
+      <c r="D77" s="2">
         <v>9.1701799999999999E-8</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:8">
       <c r="A78">
         <v>61</v>
       </c>

</xml_diff>